<commit_message>
finished Prizefighters and Game Programming Patterns
</commit_message>
<xml_diff>
--- a/report/checklist.xlsx
+++ b/report/checklist.xlsx
@@ -8,7 +8,7 @@
     <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="NEA Checklist" sheetId="1" state="visible" r:id="rId3"/>
+    <sheet name="NEA Checklist" sheetId="1" state="visible" r:id="rId2"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -932,8 +932,8 @@
   </sheetPr>
   <dimension ref="A1:H111"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A10" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A15" activeCellId="0" sqref="A15"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A25" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B32" activeCellId="0" sqref="B32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.8515625" defaultRowHeight="19.7" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -945,7 +945,7 @@
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="8" style="3" width="9.85"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="25.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -990,7 +990,7 @@
       <c r="B6" s="11"/>
       <c r="C6" s="12"/>
     </row>
-    <row r="7" customFormat="false" ht="27.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="9" t="s">
         <v>7</v>
       </c>
@@ -1003,7 +1003,7 @@
       <c r="B8" s="10"/>
       <c r="C8" s="12"/>
     </row>
-    <row r="9" customFormat="false" ht="39.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" customFormat="false" ht="27.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="9" t="s">
         <v>9</v>
       </c>
@@ -1033,18 +1033,18 @@
       </c>
       <c r="B13" s="10"/>
     </row>
-    <row r="14" customFormat="false" ht="27.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="9" t="s">
         <v>14</v>
       </c>
       <c r="B14" s="11"/>
     </row>
-    <row r="15" customFormat="false" ht="35.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="7" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="16" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="16" customFormat="false" ht="27.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A16" s="14" t="s">
         <v>16</v>
       </c>
@@ -1055,7 +1055,7 @@
       <c r="F16" s="14"/>
       <c r="G16" s="14"/>
     </row>
-    <row r="17" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="17" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A17" s="14" t="s">
         <v>17</v>
       </c>
@@ -1066,7 +1066,7 @@
       <c r="F17" s="14"/>
       <c r="G17" s="14"/>
     </row>
-    <row r="18" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="15"/>
       <c r="B18" s="15"/>
       <c r="C18" s="15"/>
@@ -1093,7 +1093,7 @@
       </c>
       <c r="B21" s="18"/>
     </row>
-    <row r="22" customFormat="false" ht="27.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="22" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="3" t="s">
         <v>21</v>
       </c>
@@ -1105,7 +1105,7 @@
       </c>
       <c r="B23" s="18"/>
     </row>
-    <row r="24" customFormat="false" ht="27.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="24" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="3" t="s">
         <v>23</v>
       </c>
@@ -1147,7 +1147,7 @@
       </c>
       <c r="B30" s="18"/>
     </row>
-    <row r="31" customFormat="false" ht="23.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="31" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B31" s="20"/>
       <c r="C31" s="20"/>
       <c r="D31" s="20"/>
@@ -1166,7 +1166,7 @@
       <c r="F32" s="21"/>
       <c r="G32" s="21"/>
     </row>
-    <row r="33" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="33" customFormat="false" ht="19.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A33" s="3" t="s">
         <v>31</v>
       </c>
@@ -1179,7 +1179,7 @@
       <c r="F33" s="22"/>
       <c r="G33" s="22"/>
     </row>
-    <row r="34" customFormat="false" ht="21" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="34" customFormat="false" ht="19.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A34" s="3" t="s">
         <v>33</v>
       </c>
@@ -1193,7 +1193,7 @@
       <c r="G34" s="22"/>
       <c r="H34" s="23"/>
     </row>
-    <row r="35" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="35" customFormat="false" ht="19.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A35" s="3" t="s">
         <v>34</v>
       </c>
@@ -1206,11 +1206,11 @@
       <c r="F35" s="22"/>
       <c r="G35" s="22"/>
     </row>
-    <row r="36" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="36" customFormat="false" ht="19.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A36" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="B36" s="18"/>
+      <c r="B36" s="19"/>
       <c r="C36" s="22" t="s">
         <v>32</v>
       </c>
@@ -1219,7 +1219,7 @@
       <c r="F36" s="22"/>
       <c r="G36" s="22"/>
     </row>
-    <row r="37" customFormat="false" ht="27.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="37" customFormat="false" ht="39.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A37" s="3" t="s">
         <v>37</v>
       </c>
@@ -1232,7 +1232,7 @@
       <c r="F37" s="22"/>
       <c r="G37" s="22"/>
     </row>
-    <row r="38" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="38" customFormat="false" ht="19.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A38" s="3" t="s">
         <v>38</v>
       </c>
@@ -1245,7 +1245,7 @@
       <c r="F38" s="24"/>
       <c r="G38" s="24"/>
     </row>
-    <row r="39" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="39" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A39" s="14" t="s">
         <v>39</v>
       </c>
@@ -1293,7 +1293,7 @@
       <c r="F42" s="22"/>
       <c r="G42" s="22"/>
     </row>
-    <row r="43" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="43" customFormat="false" ht="19.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A43" s="3" t="s">
         <v>43</v>
       </c>
@@ -1479,7 +1479,7 @@
       <c r="F59" s="22"/>
       <c r="G59" s="22"/>
     </row>
-    <row r="60" customFormat="false" ht="19.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="60" customFormat="false" ht="27.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A60" s="9" t="s">
         <v>59</v>
       </c>
@@ -1497,7 +1497,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="63" customFormat="false" ht="27.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="63" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="1" t="s">
         <v>61</v>
       </c>
@@ -1533,7 +1533,7 @@
       </c>
       <c r="B68" s="18"/>
     </row>
-    <row r="69" customFormat="false" ht="19.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="69" customFormat="false" ht="27.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A69" s="1" t="s">
         <v>65</v>
       </c>
@@ -1576,7 +1576,7 @@
       </c>
       <c r="B74" s="18"/>
     </row>
-    <row r="75" customFormat="false" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="75" customFormat="false" ht="27.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="9" t="s">
         <v>72</v>
       </c>
@@ -1588,7 +1588,7 @@
       </c>
       <c r="B76" s="18"/>
     </row>
-    <row r="77" customFormat="false" ht="27.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="77" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="9" t="s">
         <v>74</v>
       </c>
@@ -1607,7 +1607,7 @@
       <c r="F78" s="22"/>
       <c r="G78" s="22"/>
     </row>
-    <row r="79" customFormat="false" ht="19.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="79" customFormat="false" ht="27.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A79" s="9" t="s">
         <v>76</v>
       </c>
@@ -1756,7 +1756,7 @@
       </c>
       <c r="B97" s="18"/>
     </row>
-    <row r="98" customFormat="false" ht="27.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="98" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A98" s="1" t="s">
         <v>94</v>
       </c>
@@ -1792,7 +1792,7 @@
       </c>
       <c r="B103" s="18"/>
     </row>
-    <row r="104" customFormat="false" ht="52.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="104" customFormat="false" ht="39.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A104" s="1" t="s">
         <v>100</v>
       </c>

</xml_diff>

<commit_message>
start report section on prototype
</commit_message>
<xml_diff>
--- a/report/checklist.xlsx
+++ b/report/checklist.xlsx
@@ -209,7 +209,7 @@
     <t xml:space="preserve">Made prototypes of key/critical areas (if appropriate for your project)</t>
   </si>
   <si>
-    <t xml:space="preserve">List the prototypes created and section:</t>
+    <t xml:space="preserve">List the prototypes created and section: Low-level structure (Analysis/Prototyping)</t>
   </si>
   <si>
     <t xml:space="preserve">Given enough detail that a third party would understand the problem being solved/investigated</t>
@@ -933,7 +933,7 @@
   <dimension ref="A1:H111"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A25" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A37" activeCellId="0" sqref="A37"/>
+      <selection pane="topLeft" activeCell="B43" activeCellId="0" sqref="B43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.8515625" defaultRowHeight="19.7" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1170,7 +1170,7 @@
       <c r="A33" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="B33" s="18"/>
+      <c r="B33" s="19"/>
       <c r="C33" s="22" t="s">
         <v>32</v>
       </c>
@@ -1210,9 +1210,9 @@
       <c r="A36" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="B36" s="19"/>
+      <c r="B36" s="11"/>
       <c r="C36" s="22" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="D36" s="22"/>
       <c r="E36" s="22"/>
@@ -1236,7 +1236,7 @@
       <c r="A38" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="B38" s="18"/>
+      <c r="B38" s="19"/>
       <c r="C38" s="24" t="s">
         <v>32</v>
       </c>

</xml_diff>

<commit_message>
finish execution (NEA analysis deadline)
</commit_message>
<xml_diff>
--- a/report/checklist.xlsx
+++ b/report/checklist.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="114">
   <si>
     <t xml:space="preserve">Have you done the following?</t>
   </si>
@@ -188,16 +188,19 @@
     <t xml:space="preserve">Created a clear description of the problem being solved/investigated</t>
   </si>
   <si>
-    <t xml:space="preserve">Relevant Section:</t>
+    <t xml:space="preserve">Relevant Section: Description, Objectives</t>
   </si>
   <si>
     <t xml:space="preserve">Identified the end-users/supervisor that will be used in the project</t>
   </si>
   <si>
+    <t xml:space="preserve">Relevant Section: End User</t>
+  </si>
+  <si>
     <t xml:space="preserve">Researched products/software for similar problems (if appropriate for your project)</t>
   </si>
   <si>
-    <t xml:space="preserve">Relevant Section: Analysis/Research</t>
+    <t xml:space="preserve">Relevant Section: Research</t>
   </si>
   <si>
     <t xml:space="preserve">Researched relevant websites and books (if appropriate for your project)</t>
@@ -209,13 +212,19 @@
     <t xml:space="preserve">Made prototypes of key/critical areas (if appropriate for your project)</t>
   </si>
   <si>
-    <t xml:space="preserve">List the prototypes created and section: Low-level structure (Analysis/Prototyping)</t>
+    <t xml:space="preserve">Relevant Section: Prototyping</t>
+  </si>
+  <si>
+    <t xml:space="preserve">List the prototypes created and section: Low-level structure (Prototyping)</t>
   </si>
   <si>
     <t xml:space="preserve">Given enough detail that a third party would understand the problem being solved/investigated</t>
   </si>
   <si>
     <t xml:space="preserve">Added or created models/diagrams/formulae that can be used to inform the design section</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Relevant Section: Modelling</t>
   </si>
   <si>
     <r>
@@ -251,13 +260,22 @@
     </r>
   </si>
   <si>
+    <t xml:space="preserve">Relevant Section: Objectives</t>
+  </si>
+  <si>
     <t xml:space="preserve">Identified the critical-path</t>
   </si>
   <si>
+    <t xml:space="preserve">Relevant Section: Execution</t>
+  </si>
+  <si>
     <t xml:space="preserve">Documented Design</t>
   </si>
   <si>
     <t xml:space="preserve">Written an overview of how the system works</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Relevant Section:</t>
   </si>
   <si>
     <t xml:space="preserve">Given a written overview to introduce each diagram or table</t>
@@ -663,12 +681,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFC5000B"/>
-        <bgColor rgb="FF9C0006"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FF579D1C"/>
         <bgColor rgb="FF548235"/>
       </patternFill>
@@ -677,6 +689,12 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFFFD320"/>
         <bgColor rgb="FFFFFF00"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC5000B"/>
+        <bgColor rgb="FF9C0006"/>
       </patternFill>
     </fill>
   </fills>
@@ -773,14 +791,14 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="11" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="11" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -801,11 +819,11 @@
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="11" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="11" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="11" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="11" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -932,8 +950,8 @@
   </sheetPr>
   <dimension ref="A1:H111"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A25" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B43" activeCellId="0" sqref="B43"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A28" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B42" activeCellId="0" sqref="B42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.8515625" defaultRowHeight="19.7" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -974,70 +992,70 @@
       <c r="A4" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="11"/>
+      <c r="B4" s="10"/>
     </row>
     <row r="5" customFormat="false" ht="27.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="11"/>
-      <c r="C5" s="12"/>
+      <c r="B5" s="10"/>
+      <c r="C5" s="11"/>
     </row>
     <row r="6" customFormat="false" ht="27.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="B6" s="11"/>
-      <c r="C6" s="12"/>
+      <c r="B6" s="10"/>
+      <c r="C6" s="11"/>
     </row>
     <row r="7" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="B7" s="13"/>
+      <c r="B7" s="12"/>
     </row>
     <row r="8" customFormat="false" ht="27.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="9" t="s">
         <v>8</v>
       </c>
       <c r="B8" s="10"/>
-      <c r="C8" s="12"/>
+      <c r="C8" s="11"/>
     </row>
     <row r="9" customFormat="false" ht="27.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="B9" s="11"/>
+      <c r="B9" s="10"/>
     </row>
     <row r="10" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="B10" s="11"/>
+      <c r="B10" s="10"/>
     </row>
     <row r="11" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="B11" s="11"/>
+      <c r="B11" s="10"/>
     </row>
     <row r="12" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="B12" s="11"/>
+      <c r="B12" s="10"/>
     </row>
     <row r="13" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="B13" s="10"/>
+      <c r="B13" s="13"/>
     </row>
     <row r="14" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="B14" s="11"/>
+      <c r="B14" s="10"/>
     </row>
     <row r="15" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="7" t="s">
@@ -1133,13 +1151,13 @@
       <c r="A28" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="B28" s="11"/>
+      <c r="B28" s="10"/>
     </row>
     <row r="29" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="B29" s="18"/>
+      <c r="B29" s="10"/>
     </row>
     <row r="30" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="3" t="s">
@@ -1170,7 +1188,7 @@
       <c r="A33" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="B33" s="19"/>
+      <c r="B33" s="10"/>
       <c r="C33" s="22" t="s">
         <v>32</v>
       </c>
@@ -1183,9 +1201,9 @@
       <c r="A34" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="B34" s="18"/>
+      <c r="B34" s="10"/>
       <c r="C34" s="22" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="D34" s="22"/>
       <c r="E34" s="22"/>
@@ -1195,11 +1213,11 @@
     </row>
     <row r="35" customFormat="false" ht="19.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A35" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="B35" s="11"/>
+        <v>35</v>
+      </c>
+      <c r="B35" s="10"/>
       <c r="C35" s="22" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="D35" s="22"/>
       <c r="E35" s="22"/>
@@ -1208,11 +1226,11 @@
     </row>
     <row r="36" customFormat="false" ht="19.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A36" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="B36" s="10"/>
+      <c r="C36" s="22" t="s">
         <v>36</v>
-      </c>
-      <c r="B36" s="11"/>
-      <c r="C36" s="22" t="s">
-        <v>35</v>
       </c>
       <c r="D36" s="22"/>
       <c r="E36" s="22"/>
@@ -1221,11 +1239,11 @@
     </row>
     <row r="37" customFormat="false" ht="39.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A37" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="B37" s="18"/>
+        <v>38</v>
+      </c>
+      <c r="B37" s="10"/>
       <c r="C37" s="22" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="D37" s="22"/>
       <c r="E37" s="22"/>
@@ -1234,11 +1252,11 @@
     </row>
     <row r="38" customFormat="false" ht="19.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A38" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="B38" s="19"/>
+        <v>39</v>
+      </c>
+      <c r="B38" s="10"/>
       <c r="C38" s="24" t="s">
-        <v>32</v>
+        <v>40</v>
       </c>
       <c r="D38" s="24"/>
       <c r="E38" s="24"/>
@@ -1247,7 +1265,7 @@
     </row>
     <row r="39" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A39" s="14" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="B39" s="14"/>
       <c r="C39" s="14"/>
@@ -1258,9 +1276,9 @@
     </row>
     <row r="40" customFormat="false" ht="27.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="B40" s="18"/>
+        <v>42</v>
+      </c>
+      <c r="B40" s="10"/>
       <c r="C40" s="25"/>
       <c r="D40" s="25"/>
       <c r="E40" s="25"/>
@@ -1269,11 +1287,11 @@
     </row>
     <row r="41" customFormat="false" ht="19.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A41" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="B41" s="18"/>
+        <v>43</v>
+      </c>
+      <c r="B41" s="10"/>
       <c r="C41" s="22" t="s">
-        <v>32</v>
+        <v>44</v>
       </c>
       <c r="D41" s="22"/>
       <c r="E41" s="22"/>
@@ -1282,11 +1300,11 @@
     </row>
     <row r="42" customFormat="false" ht="27.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A42" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="B42" s="18"/>
+        <v>45</v>
+      </c>
+      <c r="B42" s="10"/>
       <c r="C42" s="22" t="s">
-        <v>32</v>
+        <v>46</v>
       </c>
       <c r="D42" s="22"/>
       <c r="E42" s="22"/>
@@ -1295,11 +1313,11 @@
     </row>
     <row r="43" customFormat="false" ht="19.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A43" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="B43" s="18"/>
+        <v>47</v>
+      </c>
+      <c r="B43" s="10"/>
       <c r="C43" s="22" t="s">
-        <v>32</v>
+        <v>48</v>
       </c>
       <c r="D43" s="22"/>
       <c r="E43" s="22"/>
@@ -1308,16 +1326,16 @@
     </row>
     <row r="45" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="16" t="s">
-        <v>44</v>
+        <v>49</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="19.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A46" s="9" t="s">
-        <v>45</v>
+        <v>50</v>
       </c>
       <c r="B46" s="18"/>
       <c r="C46" s="22" t="s">
-        <v>32</v>
+        <v>51</v>
       </c>
       <c r="D46" s="22"/>
       <c r="E46" s="22"/>
@@ -1326,17 +1344,17 @@
     </row>
     <row r="47" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="9" t="s">
-        <v>46</v>
+        <v>52</v>
       </c>
       <c r="B47" s="18"/>
     </row>
     <row r="48" customFormat="false" ht="19.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A48" s="9" t="s">
-        <v>47</v>
+        <v>53</v>
       </c>
       <c r="B48" s="18"/>
       <c r="C48" s="22" t="s">
-        <v>32</v>
+        <v>51</v>
       </c>
       <c r="D48" s="22"/>
       <c r="E48" s="22"/>
@@ -1345,17 +1363,17 @@
     </row>
     <row r="49" customFormat="false" ht="27.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="9" t="s">
-        <v>48</v>
+        <v>54</v>
       </c>
       <c r="B49" s="18"/>
     </row>
     <row r="50" customFormat="false" ht="19.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A50" s="9" t="s">
-        <v>49</v>
+        <v>55</v>
       </c>
       <c r="B50" s="18"/>
       <c r="C50" s="22" t="s">
-        <v>32</v>
+        <v>51</v>
       </c>
       <c r="D50" s="22"/>
       <c r="E50" s="22"/>
@@ -1364,11 +1382,11 @@
     </row>
     <row r="51" customFormat="false" ht="19.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A51" s="9" t="s">
-        <v>50</v>
+        <v>56</v>
       </c>
       <c r="B51" s="18"/>
       <c r="C51" s="22" t="s">
-        <v>32</v>
+        <v>51</v>
       </c>
       <c r="D51" s="22"/>
       <c r="E51" s="22"/>
@@ -1377,11 +1395,11 @@
     </row>
     <row r="52" customFormat="false" ht="19.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A52" s="9" t="s">
-        <v>51</v>
+        <v>57</v>
       </c>
       <c r="B52" s="18"/>
       <c r="C52" s="22" t="s">
-        <v>32</v>
+        <v>51</v>
       </c>
       <c r="D52" s="22"/>
       <c r="E52" s="22"/>
@@ -1390,11 +1408,11 @@
     </row>
     <row r="53" customFormat="false" ht="19.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A53" s="9" t="s">
-        <v>52</v>
+        <v>58</v>
       </c>
       <c r="B53" s="18"/>
       <c r="C53" s="22" t="s">
-        <v>32</v>
+        <v>51</v>
       </c>
       <c r="D53" s="22"/>
       <c r="E53" s="22"/>
@@ -1403,11 +1421,11 @@
     </row>
     <row r="54" customFormat="false" ht="19.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A54" s="9" t="s">
-        <v>53</v>
+        <v>59</v>
       </c>
       <c r="B54" s="18"/>
       <c r="C54" s="22" t="s">
-        <v>32</v>
+        <v>51</v>
       </c>
       <c r="D54" s="22"/>
       <c r="E54" s="22"/>
@@ -1416,11 +1434,11 @@
     </row>
     <row r="55" customFormat="false" ht="19.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A55" s="9" t="s">
-        <v>54</v>
+        <v>60</v>
       </c>
       <c r="B55" s="18"/>
       <c r="C55" s="22" t="s">
-        <v>32</v>
+        <v>51</v>
       </c>
       <c r="D55" s="22"/>
       <c r="E55" s="22"/>
@@ -1429,11 +1447,11 @@
     </row>
     <row r="56" customFormat="false" ht="19.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A56" s="9" t="s">
-        <v>55</v>
+        <v>61</v>
       </c>
       <c r="B56" s="18"/>
       <c r="C56" s="22" t="s">
-        <v>32</v>
+        <v>51</v>
       </c>
       <c r="D56" s="22"/>
       <c r="E56" s="22"/>
@@ -1442,11 +1460,11 @@
     </row>
     <row r="57" customFormat="false" ht="19.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A57" s="9" t="s">
-        <v>56</v>
+        <v>62</v>
       </c>
       <c r="B57" s="18"/>
       <c r="C57" s="22" t="s">
-        <v>32</v>
+        <v>51</v>
       </c>
       <c r="D57" s="22"/>
       <c r="E57" s="22"/>
@@ -1455,11 +1473,11 @@
     </row>
     <row r="58" customFormat="false" ht="19.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A58" s="9" t="s">
-        <v>57</v>
+        <v>63</v>
       </c>
       <c r="B58" s="18"/>
       <c r="C58" s="22" t="s">
-        <v>32</v>
+        <v>51</v>
       </c>
       <c r="D58" s="22"/>
       <c r="E58" s="22"/>
@@ -1468,11 +1486,11 @@
     </row>
     <row r="59" customFormat="false" ht="19.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A59" s="9" t="s">
-        <v>58</v>
+        <v>64</v>
       </c>
       <c r="B59" s="18"/>
       <c r="C59" s="22" t="s">
-        <v>32</v>
+        <v>51</v>
       </c>
       <c r="D59" s="22"/>
       <c r="E59" s="22"/>
@@ -1481,11 +1499,11 @@
     </row>
     <row r="60" customFormat="false" ht="27.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A60" s="9" t="s">
-        <v>59</v>
+        <v>65</v>
       </c>
       <c r="B60" s="18"/>
       <c r="C60" s="22" t="s">
-        <v>32</v>
+        <v>51</v>
       </c>
       <c r="D60" s="22"/>
       <c r="E60" s="22"/>
@@ -1494,30 +1512,30 @@
     </row>
     <row r="62" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="16" t="s">
-        <v>60</v>
+        <v>66</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="1" t="s">
-        <v>61</v>
+        <v>67</v>
       </c>
       <c r="B63" s="18"/>
     </row>
     <row r="64" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="9" t="s">
-        <v>62</v>
+        <v>68</v>
       </c>
       <c r="B64" s="18"/>
     </row>
     <row r="65" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="9" t="s">
-        <v>63</v>
+        <v>69</v>
       </c>
       <c r="B65" s="18"/>
     </row>
     <row r="66" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="9" t="s">
-        <v>64</v>
+        <v>70</v>
       </c>
       <c r="B66" s="18"/>
     </row>
@@ -1535,11 +1553,11 @@
     </row>
     <row r="69" customFormat="false" ht="27.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A69" s="1" t="s">
-        <v>65</v>
+        <v>71</v>
       </c>
       <c r="B69" s="18"/>
       <c r="C69" s="26" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="D69" s="26"/>
       <c r="E69" s="26"/>
@@ -1548,17 +1566,17 @@
     </row>
     <row r="70" customFormat="false" ht="27.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="1" t="s">
-        <v>67</v>
+        <v>73</v>
       </c>
       <c r="B70" s="18"/>
     </row>
     <row r="71" customFormat="false" ht="27.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A71" s="1" t="s">
-        <v>68</v>
+        <v>74</v>
       </c>
       <c r="B71" s="18"/>
       <c r="C71" s="27" t="s">
-        <v>69</v>
+        <v>75</v>
       </c>
       <c r="D71" s="27"/>
       <c r="E71" s="27"/>
@@ -1567,40 +1585,40 @@
     </row>
     <row r="73" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="16" t="s">
-        <v>70</v>
+        <v>76</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="9" t="s">
-        <v>71</v>
+        <v>77</v>
       </c>
       <c r="B74" s="18"/>
     </row>
     <row r="75" customFormat="false" ht="27.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="9" t="s">
-        <v>72</v>
+        <v>78</v>
       </c>
       <c r="B75" s="18"/>
     </row>
     <row r="76" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="9" t="s">
-        <v>73</v>
+        <v>79</v>
       </c>
       <c r="B76" s="18"/>
     </row>
     <row r="77" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="9" t="s">
-        <v>74</v>
+        <v>80</v>
       </c>
       <c r="B77" s="18"/>
     </row>
     <row r="78" customFormat="false" ht="19.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A78" s="9" t="s">
-        <v>75</v>
+        <v>81</v>
       </c>
       <c r="B78" s="18"/>
       <c r="C78" s="22" t="s">
-        <v>32</v>
+        <v>51</v>
       </c>
       <c r="D78" s="22"/>
       <c r="E78" s="22"/>
@@ -1609,11 +1627,11 @@
     </row>
     <row r="79" customFormat="false" ht="27.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A79" s="9" t="s">
-        <v>76</v>
+        <v>82</v>
       </c>
       <c r="B79" s="18"/>
       <c r="C79" s="22" t="s">
-        <v>77</v>
+        <v>83</v>
       </c>
       <c r="D79" s="22"/>
       <c r="E79" s="22"/>
@@ -1622,17 +1640,17 @@
     </row>
     <row r="80" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A80" s="9" t="s">
-        <v>78</v>
+        <v>84</v>
       </c>
       <c r="B80" s="18"/>
     </row>
     <row r="81" customFormat="false" ht="19.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A81" s="9" t="s">
-        <v>79</v>
+        <v>85</v>
       </c>
       <c r="B81" s="18"/>
       <c r="C81" s="22" t="s">
-        <v>32</v>
+        <v>51</v>
       </c>
       <c r="D81" s="22"/>
       <c r="E81" s="22"/>
@@ -1641,16 +1659,16 @@
     </row>
     <row r="83" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A83" s="16" t="s">
-        <v>80</v>
+        <v>86</v>
       </c>
     </row>
     <row r="84" customFormat="false" ht="19.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A84" s="9" t="s">
-        <v>81</v>
+        <v>87</v>
       </c>
       <c r="B84" s="18"/>
       <c r="C84" s="22" t="s">
-        <v>32</v>
+        <v>51</v>
       </c>
       <c r="D84" s="22"/>
       <c r="E84" s="22"/>
@@ -1659,11 +1677,11 @@
     </row>
     <row r="85" customFormat="false" ht="27.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A85" s="9" t="s">
-        <v>82</v>
+        <v>88</v>
       </c>
       <c r="B85" s="18"/>
       <c r="C85" s="22" t="s">
-        <v>32</v>
+        <v>51</v>
       </c>
       <c r="D85" s="22"/>
       <c r="E85" s="22"/>
@@ -1672,11 +1690,11 @@
     </row>
     <row r="86" customFormat="false" ht="19.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A86" s="9" t="s">
-        <v>83</v>
+        <v>89</v>
       </c>
       <c r="B86" s="18"/>
       <c r="C86" s="22" t="s">
-        <v>32</v>
+        <v>51</v>
       </c>
       <c r="D86" s="22"/>
       <c r="E86" s="22"/>
@@ -1685,11 +1703,11 @@
     </row>
     <row r="87" customFormat="false" ht="19.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A87" s="9" t="s">
-        <v>84</v>
+        <v>90</v>
       </c>
       <c r="B87" s="18"/>
       <c r="C87" s="22" t="s">
-        <v>32</v>
+        <v>51</v>
       </c>
       <c r="D87" s="22"/>
       <c r="E87" s="22"/>
@@ -1698,11 +1716,11 @@
     </row>
     <row r="88" customFormat="false" ht="19.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A88" s="9" t="s">
-        <v>85</v>
+        <v>91</v>
       </c>
       <c r="B88" s="18"/>
       <c r="C88" s="22" t="s">
-        <v>32</v>
+        <v>51</v>
       </c>
       <c r="D88" s="22"/>
       <c r="E88" s="22"/>
@@ -1711,132 +1729,132 @@
     </row>
     <row r="90" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A90" s="16" t="s">
-        <v>86</v>
+        <v>92</v>
       </c>
     </row>
     <row r="91" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A91" s="9" t="s">
-        <v>87</v>
+        <v>93</v>
       </c>
       <c r="B91" s="18"/>
     </row>
     <row r="92" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A92" s="9" t="s">
-        <v>88</v>
+        <v>94</v>
       </c>
       <c r="B92" s="18"/>
     </row>
     <row r="93" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A93" s="9" t="s">
-        <v>89</v>
+        <v>95</v>
       </c>
       <c r="B93" s="18"/>
     </row>
     <row r="94" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A94" s="9" t="s">
-        <v>90</v>
+        <v>96</v>
       </c>
       <c r="B94" s="18"/>
     </row>
     <row r="95" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A95" s="9" t="s">
-        <v>91</v>
+        <v>97</v>
       </c>
       <c r="B95" s="18"/>
     </row>
     <row r="96" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A96" s="9" t="s">
-        <v>92</v>
+        <v>98</v>
       </c>
       <c r="B96" s="18"/>
     </row>
     <row r="97" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A97" s="9" t="s">
-        <v>93</v>
+        <v>99</v>
       </c>
       <c r="B97" s="18"/>
     </row>
     <row r="98" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A98" s="1" t="s">
-        <v>94</v>
+        <v>100</v>
       </c>
       <c r="B98" s="18"/>
     </row>
     <row r="99" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A99" s="1" t="s">
-        <v>95</v>
+        <v>101</v>
       </c>
       <c r="B99" s="18"/>
     </row>
     <row r="100" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A100" s="1" t="s">
-        <v>96</v>
+        <v>102</v>
       </c>
       <c r="B100" s="18"/>
     </row>
     <row r="101" customFormat="false" ht="27.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A101" s="1" t="s">
-        <v>97</v>
+        <v>103</v>
       </c>
       <c r="B101" s="18"/>
     </row>
     <row r="102" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A102" s="1" t="s">
-        <v>98</v>
+        <v>104</v>
       </c>
       <c r="B102" s="18"/>
     </row>
     <row r="103" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A103" s="1" t="s">
-        <v>99</v>
+        <v>105</v>
       </c>
       <c r="B103" s="18"/>
     </row>
     <row r="104" customFormat="false" ht="39.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A104" s="1" t="s">
-        <v>100</v>
+        <v>106</v>
       </c>
       <c r="B104" s="18"/>
     </row>
     <row r="105" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A105" s="9" t="s">
-        <v>101</v>
+        <v>107</v>
       </c>
       <c r="B105" s="18"/>
     </row>
     <row r="106" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A106" s="9" t="s">
-        <v>102</v>
+        <v>108</v>
       </c>
       <c r="B106" s="18"/>
     </row>
     <row r="107" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A107" s="9" t="s">
-        <v>103</v>
+        <v>109</v>
       </c>
       <c r="B107" s="18"/>
     </row>
     <row r="108" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A108" s="9" t="s">
-        <v>104</v>
+        <v>110</v>
       </c>
       <c r="B108" s="18"/>
     </row>
     <row r="109" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A109" s="9" t="s">
-        <v>105</v>
+        <v>111</v>
       </c>
       <c r="B109" s="18"/>
     </row>
     <row r="110" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A110" s="9" t="s">
-        <v>106</v>
+        <v>112</v>
       </c>
       <c r="B110" s="18"/>
     </row>
     <row r="111" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A111" s="9" t="s">
-        <v>107</v>
+        <v>113</v>
       </c>
       <c r="B111" s="18"/>
     </row>
@@ -1879,7 +1897,7 @@
     <mergeCell ref="C87:G87"/>
     <mergeCell ref="C88:G88"/>
   </mergeCells>
-  <conditionalFormatting sqref="B2:B15 B40:B1048576 B19:B38">
+  <conditionalFormatting sqref="B40:B1048576 B2:B15 B19:B38">
     <cfRule type="containsText" priority="2" operator="containsText" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="ü" dxfId="0">
       <formula>NOT(ISERROR(SEARCH("ü",B2)))</formula>
     </cfRule>

</xml_diff>

<commit_message>
save checklist as proper xlsx file
</commit_message>
<xml_diff>
--- a/report/checklist.xlsx
+++ b/report/checklist.xlsx
@@ -2,7 +2,7 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <fileVersion appName="Calc"/>
-  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
+  <workbookPr backupFile="false" showObjects="all" dateCompatibility="false"/>
   <workbookProtection/>
   <bookViews>
     <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
@@ -950,8 +950,8 @@
   </sheetPr>
   <dimension ref="A1:H111"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A28" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B42" activeCellId="0" sqref="B42"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D9" activeCellId="0" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.8515625" defaultRowHeight="19.7" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>

<commit_message>
technical solution deadline 1
</commit_message>
<xml_diff>
--- a/report/checklist.xlsx
+++ b/report/checklist.xlsx
@@ -2,7 +2,7 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <fileVersion appName="Calc"/>
-  <workbookPr backupFile="false" showObjects="all" dateCompatibility="false"/>
+  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
     <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
@@ -687,14 +687,14 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFD320"/>
-        <bgColor rgb="FFFFFF00"/>
+        <fgColor rgb="FFC5000B"/>
+        <bgColor rgb="FF9C0006"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFC5000B"/>
-        <bgColor rgb="FF9C0006"/>
+        <fgColor rgb="FFFFD320"/>
+        <bgColor rgb="FFFFFF00"/>
       </patternFill>
     </fill>
   </fills>
@@ -746,7 +746,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="27">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -799,10 +799,6 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="11" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="165" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -819,11 +815,11 @@
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="165" fontId="11" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="165" fontId="11" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="11" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -950,8 +946,8 @@
   </sheetPr>
   <dimension ref="A1:H111"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D9" activeCellId="0" sqref="D9"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A100" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C71" activeCellId="0" sqref="C71"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.8515625" defaultRowHeight="19.7" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1012,7 +1008,7 @@
       <c r="A7" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="B7" s="12"/>
+      <c r="B7" s="10"/>
     </row>
     <row r="8" customFormat="false" ht="27.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="9" t="s">
@@ -1049,7 +1045,7 @@
       <c r="A13" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="B13" s="13"/>
+      <c r="B13" s="12"/>
     </row>
     <row r="14" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="9" t="s">
@@ -1063,89 +1059,89 @@
       </c>
     </row>
     <row r="16" customFormat="false" ht="27.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A16" s="14" t="s">
+      <c r="A16" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="B16" s="14"/>
-      <c r="C16" s="14"/>
-      <c r="D16" s="14"/>
-      <c r="E16" s="14"/>
-      <c r="F16" s="14"/>
-      <c r="G16" s="14"/>
+      <c r="B16" s="13"/>
+      <c r="C16" s="13"/>
+      <c r="D16" s="13"/>
+      <c r="E16" s="13"/>
+      <c r="F16" s="13"/>
+      <c r="G16" s="13"/>
     </row>
     <row r="17" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A17" s="14" t="s">
+      <c r="A17" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="B17" s="14"/>
-      <c r="C17" s="14"/>
-      <c r="D17" s="14"/>
-      <c r="E17" s="14"/>
-      <c r="F17" s="14"/>
-      <c r="G17" s="14"/>
+      <c r="B17" s="13"/>
+      <c r="C17" s="13"/>
+      <c r="D17" s="13"/>
+      <c r="E17" s="13"/>
+      <c r="F17" s="13"/>
+      <c r="G17" s="13"/>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="15"/>
-      <c r="B18" s="15"/>
-      <c r="C18" s="15"/>
-      <c r="D18" s="15"/>
-      <c r="E18" s="15"/>
-      <c r="F18" s="15"/>
-      <c r="G18" s="15"/>
+      <c r="A18" s="14"/>
+      <c r="B18" s="14"/>
+      <c r="C18" s="14"/>
+      <c r="D18" s="14"/>
+      <c r="E18" s="14"/>
+      <c r="F18" s="14"/>
+      <c r="G18" s="14"/>
     </row>
     <row r="19" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="16" t="s">
+      <c r="A19" s="15" t="s">
         <v>18</v>
       </c>
-      <c r="B19" s="17"/>
+      <c r="B19" s="16"/>
     </row>
     <row r="20" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="B20" s="18"/>
+      <c r="B20" s="17"/>
     </row>
     <row r="21" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="B21" s="18"/>
+      <c r="B21" s="17"/>
     </row>
     <row r="22" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="B22" s="18"/>
+      <c r="B22" s="17"/>
     </row>
     <row r="23" customFormat="false" ht="27.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="B23" s="18"/>
+      <c r="B23" s="17"/>
     </row>
     <row r="24" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="B24" s="19"/>
+      <c r="B24" s="18"/>
     </row>
     <row r="25" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="B25" s="18"/>
+      <c r="B25" s="17"/>
     </row>
     <row r="26" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="B26" s="18"/>
+      <c r="B26" s="17"/>
     </row>
     <row r="27" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="B27" s="18"/>
+      <c r="B27" s="17"/>
     </row>
     <row r="28" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="3" t="s">
@@ -1163,169 +1159,169 @@
       <c r="A30" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="B30" s="18"/>
+      <c r="B30" s="17"/>
     </row>
     <row r="31" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B31" s="20"/>
-      <c r="C31" s="20"/>
-      <c r="D31" s="20"/>
-      <c r="E31" s="20"/>
-      <c r="F31" s="20"/>
-      <c r="G31" s="20"/>
+      <c r="B31" s="19"/>
+      <c r="C31" s="19"/>
+      <c r="D31" s="19"/>
+      <c r="E31" s="19"/>
+      <c r="F31" s="19"/>
+      <c r="G31" s="19"/>
     </row>
     <row r="32" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="16" t="s">
+      <c r="A32" s="15" t="s">
         <v>30</v>
       </c>
-      <c r="B32" s="21"/>
-      <c r="C32" s="21"/>
-      <c r="D32" s="21"/>
-      <c r="E32" s="21"/>
-      <c r="F32" s="21"/>
-      <c r="G32" s="21"/>
+      <c r="B32" s="20"/>
+      <c r="C32" s="20"/>
+      <c r="D32" s="20"/>
+      <c r="E32" s="20"/>
+      <c r="F32" s="20"/>
+      <c r="G32" s="20"/>
     </row>
     <row r="33" customFormat="false" ht="19.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A33" s="3" t="s">
         <v>31</v>
       </c>
       <c r="B33" s="10"/>
-      <c r="C33" s="22" t="s">
+      <c r="C33" s="21" t="s">
         <v>32</v>
       </c>
-      <c r="D33" s="22"/>
-      <c r="E33" s="22"/>
-      <c r="F33" s="22"/>
-      <c r="G33" s="22"/>
+      <c r="D33" s="21"/>
+      <c r="E33" s="21"/>
+      <c r="F33" s="21"/>
+      <c r="G33" s="21"/>
     </row>
     <row r="34" customFormat="false" ht="19.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A34" s="3" t="s">
         <v>33</v>
       </c>
       <c r="B34" s="10"/>
-      <c r="C34" s="22" t="s">
+      <c r="C34" s="21" t="s">
         <v>34</v>
       </c>
-      <c r="D34" s="22"/>
-      <c r="E34" s="22"/>
-      <c r="F34" s="22"/>
-      <c r="G34" s="22"/>
-      <c r="H34" s="23"/>
+      <c r="D34" s="21"/>
+      <c r="E34" s="21"/>
+      <c r="F34" s="21"/>
+      <c r="G34" s="21"/>
+      <c r="H34" s="22"/>
     </row>
     <row r="35" customFormat="false" ht="19.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A35" s="3" t="s">
         <v>35</v>
       </c>
       <c r="B35" s="10"/>
-      <c r="C35" s="22" t="s">
+      <c r="C35" s="21" t="s">
         <v>36</v>
       </c>
-      <c r="D35" s="22"/>
-      <c r="E35" s="22"/>
-      <c r="F35" s="22"/>
-      <c r="G35" s="22"/>
+      <c r="D35" s="21"/>
+      <c r="E35" s="21"/>
+      <c r="F35" s="21"/>
+      <c r="G35" s="21"/>
     </row>
     <row r="36" customFormat="false" ht="19.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A36" s="3" t="s">
         <v>37</v>
       </c>
       <c r="B36" s="10"/>
-      <c r="C36" s="22" t="s">
+      <c r="C36" s="21" t="s">
         <v>36</v>
       </c>
-      <c r="D36" s="22"/>
-      <c r="E36" s="22"/>
-      <c r="F36" s="22"/>
-      <c r="G36" s="22"/>
+      <c r="D36" s="21"/>
+      <c r="E36" s="21"/>
+      <c r="F36" s="21"/>
+      <c r="G36" s="21"/>
     </row>
     <row r="37" customFormat="false" ht="39.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A37" s="3" t="s">
         <v>38</v>
       </c>
       <c r="B37" s="10"/>
-      <c r="C37" s="22" t="s">
+      <c r="C37" s="21" t="s">
         <v>34</v>
       </c>
-      <c r="D37" s="22"/>
-      <c r="E37" s="22"/>
-      <c r="F37" s="22"/>
-      <c r="G37" s="22"/>
+      <c r="D37" s="21"/>
+      <c r="E37" s="21"/>
+      <c r="F37" s="21"/>
+      <c r="G37" s="21"/>
     </row>
     <row r="38" customFormat="false" ht="19.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A38" s="3" t="s">
         <v>39</v>
       </c>
       <c r="B38" s="10"/>
-      <c r="C38" s="24" t="s">
+      <c r="C38" s="23" t="s">
         <v>40</v>
       </c>
-      <c r="D38" s="24"/>
-      <c r="E38" s="24"/>
-      <c r="F38" s="24"/>
-      <c r="G38" s="24"/>
+      <c r="D38" s="23"/>
+      <c r="E38" s="23"/>
+      <c r="F38" s="23"/>
+      <c r="G38" s="23"/>
     </row>
     <row r="39" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A39" s="14" t="s">
+      <c r="A39" s="13" t="s">
         <v>41</v>
       </c>
-      <c r="B39" s="14"/>
-      <c r="C39" s="14"/>
-      <c r="D39" s="14"/>
-      <c r="E39" s="14"/>
-      <c r="F39" s="14"/>
-      <c r="G39" s="14"/>
+      <c r="B39" s="13"/>
+      <c r="C39" s="13"/>
+      <c r="D39" s="13"/>
+      <c r="E39" s="13"/>
+      <c r="F39" s="13"/>
+      <c r="G39" s="13"/>
     </row>
     <row r="40" customFormat="false" ht="27.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="3" t="s">
         <v>42</v>
       </c>
       <c r="B40" s="10"/>
-      <c r="C40" s="25"/>
-      <c r="D40" s="25"/>
-      <c r="E40" s="25"/>
-      <c r="F40" s="25"/>
-      <c r="G40" s="25"/>
+      <c r="C40" s="24"/>
+      <c r="D40" s="24"/>
+      <c r="E40" s="24"/>
+      <c r="F40" s="24"/>
+      <c r="G40" s="24"/>
     </row>
     <row r="41" customFormat="false" ht="19.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A41" s="3" t="s">
         <v>43</v>
       </c>
       <c r="B41" s="10"/>
-      <c r="C41" s="22" t="s">
+      <c r="C41" s="21" t="s">
         <v>44</v>
       </c>
-      <c r="D41" s="22"/>
-      <c r="E41" s="22"/>
-      <c r="F41" s="22"/>
-      <c r="G41" s="22"/>
+      <c r="D41" s="21"/>
+      <c r="E41" s="21"/>
+      <c r="F41" s="21"/>
+      <c r="G41" s="21"/>
     </row>
     <row r="42" customFormat="false" ht="27.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A42" s="3" t="s">
         <v>45</v>
       </c>
       <c r="B42" s="10"/>
-      <c r="C42" s="22" t="s">
+      <c r="C42" s="21" t="s">
         <v>46</v>
       </c>
-      <c r="D42" s="22"/>
-      <c r="E42" s="22"/>
-      <c r="F42" s="22"/>
-      <c r="G42" s="22"/>
+      <c r="D42" s="21"/>
+      <c r="E42" s="21"/>
+      <c r="F42" s="21"/>
+      <c r="G42" s="21"/>
     </row>
     <row r="43" customFormat="false" ht="19.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A43" s="3" t="s">
         <v>47</v>
       </c>
       <c r="B43" s="10"/>
-      <c r="C43" s="22" t="s">
+      <c r="C43" s="21" t="s">
         <v>48</v>
       </c>
-      <c r="D43" s="22"/>
-      <c r="E43" s="22"/>
-      <c r="F43" s="22"/>
-      <c r="G43" s="22"/>
+      <c r="D43" s="21"/>
+      <c r="E43" s="21"/>
+      <c r="F43" s="21"/>
+      <c r="G43" s="21"/>
     </row>
     <row r="45" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A45" s="16" t="s">
+      <c r="A45" s="15" t="s">
         <v>49</v>
       </c>
     </row>
@@ -1334,184 +1330,184 @@
         <v>50</v>
       </c>
       <c r="B46" s="18"/>
-      <c r="C46" s="22" t="s">
+      <c r="C46" s="21" t="s">
         <v>51</v>
       </c>
-      <c r="D46" s="22"/>
-      <c r="E46" s="22"/>
-      <c r="F46" s="22"/>
-      <c r="G46" s="22"/>
+      <c r="D46" s="21"/>
+      <c r="E46" s="21"/>
+      <c r="F46" s="21"/>
+      <c r="G46" s="21"/>
     </row>
     <row r="47" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="9" t="s">
         <v>52</v>
       </c>
-      <c r="B47" s="18"/>
+      <c r="B47" s="17"/>
     </row>
     <row r="48" customFormat="false" ht="19.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A48" s="9" t="s">
         <v>53</v>
       </c>
       <c r="B48" s="18"/>
-      <c r="C48" s="22" t="s">
+      <c r="C48" s="21" t="s">
         <v>51</v>
       </c>
-      <c r="D48" s="22"/>
-      <c r="E48" s="22"/>
-      <c r="F48" s="22"/>
-      <c r="G48" s="22"/>
+      <c r="D48" s="21"/>
+      <c r="E48" s="21"/>
+      <c r="F48" s="21"/>
+      <c r="G48" s="21"/>
     </row>
     <row r="49" customFormat="false" ht="27.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="9" t="s">
         <v>54</v>
       </c>
-      <c r="B49" s="18"/>
+      <c r="B49" s="17"/>
     </row>
     <row r="50" customFormat="false" ht="19.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A50" s="9" t="s">
         <v>55</v>
       </c>
-      <c r="B50" s="18"/>
-      <c r="C50" s="22" t="s">
+      <c r="B50" s="17"/>
+      <c r="C50" s="21" t="s">
         <v>51</v>
       </c>
-      <c r="D50" s="22"/>
-      <c r="E50" s="22"/>
-      <c r="F50" s="22"/>
-      <c r="G50" s="22"/>
+      <c r="D50" s="21"/>
+      <c r="E50" s="21"/>
+      <c r="F50" s="21"/>
+      <c r="G50" s="21"/>
     </row>
     <row r="51" customFormat="false" ht="19.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A51" s="9" t="s">
         <v>56</v>
       </c>
-      <c r="B51" s="18"/>
-      <c r="C51" s="22" t="s">
+      <c r="B51" s="17"/>
+      <c r="C51" s="21" t="s">
         <v>51</v>
       </c>
-      <c r="D51" s="22"/>
-      <c r="E51" s="22"/>
-      <c r="F51" s="22"/>
-      <c r="G51" s="22"/>
+      <c r="D51" s="21"/>
+      <c r="E51" s="21"/>
+      <c r="F51" s="21"/>
+      <c r="G51" s="21"/>
     </row>
     <row r="52" customFormat="false" ht="19.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A52" s="9" t="s">
         <v>57</v>
       </c>
-      <c r="B52" s="18"/>
-      <c r="C52" s="22" t="s">
+      <c r="B52" s="17"/>
+      <c r="C52" s="21" t="s">
         <v>51</v>
       </c>
-      <c r="D52" s="22"/>
-      <c r="E52" s="22"/>
-      <c r="F52" s="22"/>
-      <c r="G52" s="22"/>
+      <c r="D52" s="21"/>
+      <c r="E52" s="21"/>
+      <c r="F52" s="21"/>
+      <c r="G52" s="21"/>
     </row>
     <row r="53" customFormat="false" ht="19.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A53" s="9" t="s">
         <v>58</v>
       </c>
-      <c r="B53" s="18"/>
-      <c r="C53" s="22" t="s">
+      <c r="B53" s="17"/>
+      <c r="C53" s="21" t="s">
         <v>51</v>
       </c>
-      <c r="D53" s="22"/>
-      <c r="E53" s="22"/>
-      <c r="F53" s="22"/>
-      <c r="G53" s="22"/>
+      <c r="D53" s="21"/>
+      <c r="E53" s="21"/>
+      <c r="F53" s="21"/>
+      <c r="G53" s="21"/>
     </row>
     <row r="54" customFormat="false" ht="19.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A54" s="9" t="s">
         <v>59</v>
       </c>
-      <c r="B54" s="18"/>
-      <c r="C54" s="22" t="s">
+      <c r="B54" s="17"/>
+      <c r="C54" s="21" t="s">
         <v>51</v>
       </c>
-      <c r="D54" s="22"/>
-      <c r="E54" s="22"/>
-      <c r="F54" s="22"/>
-      <c r="G54" s="22"/>
+      <c r="D54" s="21"/>
+      <c r="E54" s="21"/>
+      <c r="F54" s="21"/>
+      <c r="G54" s="21"/>
     </row>
     <row r="55" customFormat="false" ht="19.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A55" s="9" t="s">
         <v>60</v>
       </c>
-      <c r="B55" s="18"/>
-      <c r="C55" s="22" t="s">
+      <c r="B55" s="17"/>
+      <c r="C55" s="21" t="s">
         <v>51</v>
       </c>
-      <c r="D55" s="22"/>
-      <c r="E55" s="22"/>
-      <c r="F55" s="22"/>
-      <c r="G55" s="22"/>
+      <c r="D55" s="21"/>
+      <c r="E55" s="21"/>
+      <c r="F55" s="21"/>
+      <c r="G55" s="21"/>
     </row>
     <row r="56" customFormat="false" ht="19.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A56" s="9" t="s">
         <v>61</v>
       </c>
-      <c r="B56" s="18"/>
-      <c r="C56" s="22" t="s">
+      <c r="B56" s="17"/>
+      <c r="C56" s="21" t="s">
         <v>51</v>
       </c>
-      <c r="D56" s="22"/>
-      <c r="E56" s="22"/>
-      <c r="F56" s="22"/>
-      <c r="G56" s="22"/>
+      <c r="D56" s="21"/>
+      <c r="E56" s="21"/>
+      <c r="F56" s="21"/>
+      <c r="G56" s="21"/>
     </row>
     <row r="57" customFormat="false" ht="19.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A57" s="9" t="s">
         <v>62</v>
       </c>
-      <c r="B57" s="18"/>
-      <c r="C57" s="22" t="s">
+      <c r="B57" s="17"/>
+      <c r="C57" s="21" t="s">
         <v>51</v>
       </c>
-      <c r="D57" s="22"/>
-      <c r="E57" s="22"/>
-      <c r="F57" s="22"/>
-      <c r="G57" s="22"/>
+      <c r="D57" s="21"/>
+      <c r="E57" s="21"/>
+      <c r="F57" s="21"/>
+      <c r="G57" s="21"/>
     </row>
     <row r="58" customFormat="false" ht="19.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A58" s="9" t="s">
         <v>63</v>
       </c>
-      <c r="B58" s="18"/>
-      <c r="C58" s="22" t="s">
+      <c r="B58" s="17"/>
+      <c r="C58" s="21" t="s">
         <v>51</v>
       </c>
-      <c r="D58" s="22"/>
-      <c r="E58" s="22"/>
-      <c r="F58" s="22"/>
-      <c r="G58" s="22"/>
+      <c r="D58" s="21"/>
+      <c r="E58" s="21"/>
+      <c r="F58" s="21"/>
+      <c r="G58" s="21"/>
     </row>
     <row r="59" customFormat="false" ht="19.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A59" s="9" t="s">
         <v>64</v>
       </c>
-      <c r="B59" s="18"/>
-      <c r="C59" s="22" t="s">
+      <c r="B59" s="17"/>
+      <c r="C59" s="21" t="s">
         <v>51</v>
       </c>
-      <c r="D59" s="22"/>
-      <c r="E59" s="22"/>
-      <c r="F59" s="22"/>
-      <c r="G59" s="22"/>
+      <c r="D59" s="21"/>
+      <c r="E59" s="21"/>
+      <c r="F59" s="21"/>
+      <c r="G59" s="21"/>
     </row>
     <row r="60" customFormat="false" ht="27.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A60" s="9" t="s">
         <v>65</v>
       </c>
-      <c r="B60" s="18"/>
-      <c r="C60" s="22" t="s">
+      <c r="B60" s="17"/>
+      <c r="C60" s="21" t="s">
         <v>51</v>
       </c>
-      <c r="D60" s="22"/>
-      <c r="E60" s="22"/>
-      <c r="F60" s="22"/>
-      <c r="G60" s="22"/>
+      <c r="D60" s="21"/>
+      <c r="E60" s="21"/>
+      <c r="F60" s="21"/>
+      <c r="G60" s="21"/>
     </row>
     <row r="62" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A62" s="16" t="s">
+      <c r="A62" s="15" t="s">
         <v>66</v>
       </c>
     </row>
@@ -1525,44 +1521,44 @@
       <c r="A64" s="9" t="s">
         <v>68</v>
       </c>
-      <c r="B64" s="18"/>
+      <c r="B64" s="17"/>
     </row>
     <row r="65" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="9" t="s">
         <v>69</v>
       </c>
-      <c r="B65" s="18"/>
+      <c r="B65" s="17"/>
     </row>
     <row r="66" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="9" t="s">
         <v>70</v>
       </c>
-      <c r="B66" s="18"/>
+      <c r="B66" s="17"/>
     </row>
     <row r="67" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="B67" s="18"/>
+      <c r="B67" s="17"/>
     </row>
     <row r="68" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="B68" s="18"/>
+      <c r="B68" s="17"/>
     </row>
     <row r="69" customFormat="false" ht="27.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A69" s="1" t="s">
         <v>71</v>
       </c>
       <c r="B69" s="18"/>
-      <c r="C69" s="26" t="s">
+      <c r="C69" s="25" t="s">
         <v>72</v>
       </c>
-      <c r="D69" s="26"/>
-      <c r="E69" s="26"/>
-      <c r="F69" s="26"/>
-      <c r="G69" s="26"/>
+      <c r="D69" s="25"/>
+      <c r="E69" s="25"/>
+      <c r="F69" s="25"/>
+      <c r="G69" s="25"/>
     </row>
     <row r="70" customFormat="false" ht="27.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="1" t="s">
@@ -1574,17 +1570,17 @@
       <c r="A71" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="B71" s="18"/>
-      <c r="C71" s="27" t="s">
+      <c r="B71" s="17"/>
+      <c r="C71" s="26" t="s">
         <v>75</v>
       </c>
-      <c r="D71" s="27"/>
-      <c r="E71" s="27"/>
-      <c r="F71" s="27"/>
-      <c r="G71" s="27"/>
+      <c r="D71" s="26"/>
+      <c r="E71" s="26"/>
+      <c r="F71" s="26"/>
+      <c r="G71" s="26"/>
     </row>
     <row r="73" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A73" s="16" t="s">
+      <c r="A73" s="15" t="s">
         <v>76</v>
       </c>
     </row>
@@ -1592,73 +1588,73 @@
       <c r="A74" s="9" t="s">
         <v>77</v>
       </c>
-      <c r="B74" s="18"/>
+      <c r="B74" s="17"/>
     </row>
     <row r="75" customFormat="false" ht="27.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="9" t="s">
         <v>78</v>
       </c>
-      <c r="B75" s="18"/>
+      <c r="B75" s="17"/>
     </row>
     <row r="76" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="9" t="s">
         <v>79</v>
       </c>
-      <c r="B76" s="18"/>
+      <c r="B76" s="17"/>
     </row>
     <row r="77" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="9" t="s">
         <v>80</v>
       </c>
-      <c r="B77" s="18"/>
+      <c r="B77" s="17"/>
     </row>
     <row r="78" customFormat="false" ht="19.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A78" s="9" t="s">
         <v>81</v>
       </c>
-      <c r="B78" s="18"/>
-      <c r="C78" s="22" t="s">
+      <c r="B78" s="17"/>
+      <c r="C78" s="21" t="s">
         <v>51</v>
       </c>
-      <c r="D78" s="22"/>
-      <c r="E78" s="22"/>
-      <c r="F78" s="22"/>
-      <c r="G78" s="22"/>
+      <c r="D78" s="21"/>
+      <c r="E78" s="21"/>
+      <c r="F78" s="21"/>
+      <c r="G78" s="21"/>
     </row>
     <row r="79" customFormat="false" ht="27.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A79" s="9" t="s">
         <v>82</v>
       </c>
-      <c r="B79" s="18"/>
-      <c r="C79" s="22" t="s">
+      <c r="B79" s="17"/>
+      <c r="C79" s="21" t="s">
         <v>83</v>
       </c>
-      <c r="D79" s="22"/>
-      <c r="E79" s="22"/>
-      <c r="F79" s="22"/>
-      <c r="G79" s="22"/>
+      <c r="D79" s="21"/>
+      <c r="E79" s="21"/>
+      <c r="F79" s="21"/>
+      <c r="G79" s="21"/>
     </row>
     <row r="80" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A80" s="9" t="s">
         <v>84</v>
       </c>
-      <c r="B80" s="18"/>
+      <c r="B80" s="17"/>
     </row>
     <row r="81" customFormat="false" ht="19.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A81" s="9" t="s">
         <v>85</v>
       </c>
-      <c r="B81" s="18"/>
-      <c r="C81" s="22" t="s">
+      <c r="B81" s="17"/>
+      <c r="C81" s="21" t="s">
         <v>51</v>
       </c>
-      <c r="D81" s="22"/>
-      <c r="E81" s="22"/>
-      <c r="F81" s="22"/>
-      <c r="G81" s="22"/>
+      <c r="D81" s="21"/>
+      <c r="E81" s="21"/>
+      <c r="F81" s="21"/>
+      <c r="G81" s="21"/>
     </row>
     <row r="83" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A83" s="16" t="s">
+      <c r="A83" s="15" t="s">
         <v>86</v>
       </c>
     </row>
@@ -1666,69 +1662,69 @@
       <c r="A84" s="9" t="s">
         <v>87</v>
       </c>
-      <c r="B84" s="18"/>
-      <c r="C84" s="22" t="s">
+      <c r="B84" s="17"/>
+      <c r="C84" s="21" t="s">
         <v>51</v>
       </c>
-      <c r="D84" s="22"/>
-      <c r="E84" s="22"/>
-      <c r="F84" s="22"/>
-      <c r="G84" s="22"/>
+      <c r="D84" s="21"/>
+      <c r="E84" s="21"/>
+      <c r="F84" s="21"/>
+      <c r="G84" s="21"/>
     </row>
     <row r="85" customFormat="false" ht="27.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A85" s="9" t="s">
         <v>88</v>
       </c>
-      <c r="B85" s="18"/>
-      <c r="C85" s="22" t="s">
+      <c r="B85" s="17"/>
+      <c r="C85" s="21" t="s">
         <v>51</v>
       </c>
-      <c r="D85" s="22"/>
-      <c r="E85" s="22"/>
-      <c r="F85" s="22"/>
-      <c r="G85" s="22"/>
+      <c r="D85" s="21"/>
+      <c r="E85" s="21"/>
+      <c r="F85" s="21"/>
+      <c r="G85" s="21"/>
     </row>
     <row r="86" customFormat="false" ht="19.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A86" s="9" t="s">
         <v>89</v>
       </c>
-      <c r="B86" s="18"/>
-      <c r="C86" s="22" t="s">
+      <c r="B86" s="17"/>
+      <c r="C86" s="21" t="s">
         <v>51</v>
       </c>
-      <c r="D86" s="22"/>
-      <c r="E86" s="22"/>
-      <c r="F86" s="22"/>
-      <c r="G86" s="22"/>
+      <c r="D86" s="21"/>
+      <c r="E86" s="21"/>
+      <c r="F86" s="21"/>
+      <c r="G86" s="21"/>
     </row>
     <row r="87" customFormat="false" ht="19.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A87" s="9" t="s">
         <v>90</v>
       </c>
-      <c r="B87" s="18"/>
-      <c r="C87" s="22" t="s">
+      <c r="B87" s="17"/>
+      <c r="C87" s="21" t="s">
         <v>51</v>
       </c>
-      <c r="D87" s="22"/>
-      <c r="E87" s="22"/>
-      <c r="F87" s="22"/>
-      <c r="G87" s="22"/>
+      <c r="D87" s="21"/>
+      <c r="E87" s="21"/>
+      <c r="F87" s="21"/>
+      <c r="G87" s="21"/>
     </row>
     <row r="88" customFormat="false" ht="19.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A88" s="9" t="s">
         <v>91</v>
       </c>
-      <c r="B88" s="18"/>
-      <c r="C88" s="22" t="s">
+      <c r="B88" s="17"/>
+      <c r="C88" s="21" t="s">
         <v>51</v>
       </c>
-      <c r="D88" s="22"/>
-      <c r="E88" s="22"/>
-      <c r="F88" s="22"/>
-      <c r="G88" s="22"/>
+      <c r="D88" s="21"/>
+      <c r="E88" s="21"/>
+      <c r="F88" s="21"/>
+      <c r="G88" s="21"/>
     </row>
     <row r="90" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A90" s="16" t="s">
+      <c r="A90" s="15" t="s">
         <v>92</v>
       </c>
     </row>
@@ -1736,127 +1732,127 @@
       <c r="A91" s="9" t="s">
         <v>93</v>
       </c>
-      <c r="B91" s="18"/>
+      <c r="B91" s="17"/>
     </row>
     <row r="92" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A92" s="9" t="s">
         <v>94</v>
       </c>
-      <c r="B92" s="18"/>
+      <c r="B92" s="17"/>
     </row>
     <row r="93" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A93" s="9" t="s">
         <v>95</v>
       </c>
-      <c r="B93" s="18"/>
+      <c r="B93" s="17"/>
     </row>
     <row r="94" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A94" s="9" t="s">
         <v>96</v>
       </c>
-      <c r="B94" s="18"/>
+      <c r="B94" s="17"/>
     </row>
     <row r="95" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A95" s="9" t="s">
         <v>97</v>
       </c>
-      <c r="B95" s="18"/>
+      <c r="B95" s="17"/>
     </row>
     <row r="96" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A96" s="9" t="s">
         <v>98</v>
       </c>
-      <c r="B96" s="18"/>
+      <c r="B96" s="17"/>
     </row>
     <row r="97" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A97" s="9" t="s">
         <v>99</v>
       </c>
-      <c r="B97" s="18"/>
+      <c r="B97" s="17"/>
     </row>
     <row r="98" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A98" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="B98" s="18"/>
+      <c r="B98" s="17"/>
     </row>
     <row r="99" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A99" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="B99" s="18"/>
+      <c r="B99" s="17"/>
     </row>
     <row r="100" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A100" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="B100" s="18"/>
+      <c r="B100" s="17"/>
     </row>
     <row r="101" customFormat="false" ht="27.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A101" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="B101" s="18"/>
+      <c r="B101" s="17"/>
     </row>
     <row r="102" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A102" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="B102" s="18"/>
+      <c r="B102" s="17"/>
     </row>
     <row r="103" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A103" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="B103" s="18"/>
+      <c r="B103" s="17"/>
     </row>
     <row r="104" customFormat="false" ht="39.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A104" s="1" t="s">
         <v>106</v>
       </c>
-      <c r="B104" s="18"/>
+      <c r="B104" s="17"/>
     </row>
     <row r="105" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A105" s="9" t="s">
         <v>107</v>
       </c>
-      <c r="B105" s="18"/>
+      <c r="B105" s="17"/>
     </row>
     <row r="106" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A106" s="9" t="s">
         <v>108</v>
       </c>
-      <c r="B106" s="18"/>
+      <c r="B106" s="17"/>
     </row>
     <row r="107" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A107" s="9" t="s">
         <v>109</v>
       </c>
-      <c r="B107" s="18"/>
+      <c r="B107" s="17"/>
     </row>
     <row r="108" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A108" s="9" t="s">
         <v>110</v>
       </c>
-      <c r="B108" s="18"/>
+      <c r="B108" s="17"/>
     </row>
     <row r="109" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A109" s="9" t="s">
         <v>111</v>
       </c>
-      <c r="B109" s="18"/>
+      <c r="B109" s="17"/>
     </row>
     <row r="110" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A110" s="9" t="s">
         <v>112</v>
       </c>
-      <c r="B110" s="18"/>
+      <c r="B110" s="17"/>
     </row>
     <row r="111" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A111" s="9" t="s">
         <v>113</v>
       </c>
-      <c r="B111" s="18"/>
+      <c r="B111" s="17"/>
     </row>
   </sheetData>
   <mergeCells count="36">
@@ -1897,7 +1893,7 @@
     <mergeCell ref="C87:G87"/>
     <mergeCell ref="C88:G88"/>
   </mergeCells>
-  <conditionalFormatting sqref="B40:B1048576 B2:B15 B19:B38">
+  <conditionalFormatting sqref="B19:B38 B2:B15 B40:B1048576">
     <cfRule type="containsText" priority="2" operator="containsText" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="ü" dxfId="0">
       <formula>NOT(ISERROR(SEARCH("ü",B2)))</formula>
     </cfRule>
@@ -1906,7 +1902,7 @@
     </cfRule>
   </conditionalFormatting>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>

</xml_diff>

<commit_message>
fix objectives ticks and update checklist
</commit_message>
<xml_diff>
--- a/report/checklist.xlsx
+++ b/report/checklist.xlsx
@@ -347,7 +347,7 @@
     <t xml:space="preserve">Demonstrated the completeness of the solution compared to the objectives created in the Documented Design section.</t>
   </si>
   <si>
-    <t xml:space="preserve">List incomplete core-objectives here.</t>
+    <t xml:space="preserve">See Technical Solution/Objectives</t>
   </si>
   <si>
     <t xml:space="preserve">Testing</t>
@@ -946,8 +946,8 @@
   </sheetPr>
   <dimension ref="A1:H111"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A100" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C71" activeCellId="0" sqref="C71"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A61" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A72" activeCellId="0" sqref="A72"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.8515625" defaultRowHeight="19.7" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1515,13 +1515,13 @@
       <c r="A63" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="B63" s="18"/>
+      <c r="B63" s="10"/>
     </row>
     <row r="64" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="9" t="s">
         <v>68</v>
       </c>
-      <c r="B64" s="17"/>
+      <c r="B64" s="10"/>
     </row>
     <row r="65" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="9" t="s">
@@ -1533,7 +1533,7 @@
       <c r="A66" s="9" t="s">
         <v>70</v>
       </c>
-      <c r="B66" s="17"/>
+      <c r="B66" s="10"/>
     </row>
     <row r="67" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="3" t="s">
@@ -1564,13 +1564,13 @@
       <c r="A70" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="B70" s="18"/>
+      <c r="B70" s="10"/>
     </row>
     <row r="71" customFormat="false" ht="27.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A71" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="B71" s="17"/>
+      <c r="B71" s="10"/>
       <c r="C71" s="26" t="s">
         <v>75</v>
       </c>

</xml_diff>

<commit_message>
describe launchers and initialisation of main class
</commit_message>
<xml_diff>
--- a/report/checklist.xlsx
+++ b/report/checklist.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="114">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="115">
   <si>
     <t xml:space="preserve">Have you done the following?</t>
   </si>
@@ -297,6 +297,9 @@
   </si>
   <si>
     <t xml:space="preserve">If using a database, created the database design</t>
+  </si>
+  <si>
+    <t xml:space="preserve">N/A</t>
   </si>
   <si>
     <t xml:space="preserve">If using a database, created the database queries</t>
@@ -564,7 +567,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="@"/>
   </numFmts>
-  <fonts count="15">
+  <fonts count="17">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -599,7 +602,7 @@
       <b val="true"/>
       <sz val="16"/>
       <color rgb="FF000000"/>
-      <name val="Arial Nova"/>
+      <name val="Noto Sans"/>
       <family val="2"/>
       <charset val="1"/>
     </font>
@@ -642,14 +645,6 @@
       <charset val="1"/>
     </font>
     <font>
-      <b val="true"/>
-      <sz val="16"/>
-      <color rgb="FF000000"/>
-      <name val="Wingdings"/>
-      <family val="0"/>
-      <charset val="2"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Wingdings"/>
@@ -657,10 +652,34 @@
       <charset val="2"/>
     </font>
     <font>
+      <b val="true"/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Noto Sans"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="16"/>
+      <color rgb="FF000000"/>
+      <name val="Arial Nova"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Courier New"/>
       <family val="3"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="14"/>
+      <color rgb="FFFF0000"/>
+      <name val="Noto Sans"/>
+      <family val="2"/>
       <charset val="1"/>
     </font>
     <font>
@@ -746,7 +765,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="30">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -779,23 +798,19 @@
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="165" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="11" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="11" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -807,23 +822,31 @@
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="165" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="165" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="11" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="11" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -831,11 +854,15 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -845,6 +872,10 @@
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
@@ -946,8 +977,8 @@
   </sheetPr>
   <dimension ref="A1:H111"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A61" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A72" activeCellId="0" sqref="A72"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A43" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A60" activeCellId="0" sqref="A60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.8515625" defaultRowHeight="19.7" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -976,82 +1007,81 @@
       <c r="A2" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="8"/>
     </row>
     <row r="3" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="9" t="s">
+      <c r="A3" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="10"/>
+      <c r="B3" s="9"/>
     </row>
     <row r="4" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="9" t="s">
+      <c r="A4" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="10"/>
+      <c r="B4" s="9"/>
     </row>
     <row r="5" customFormat="false" ht="27.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="9" t="s">
+      <c r="A5" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="10"/>
-      <c r="C5" s="11"/>
+      <c r="B5" s="9"/>
+      <c r="C5" s="10"/>
     </row>
     <row r="6" customFormat="false" ht="27.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="9" t="s">
+      <c r="A6" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="B6" s="10"/>
-      <c r="C6" s="11"/>
+      <c r="B6" s="9"/>
+      <c r="C6" s="10"/>
     </row>
     <row r="7" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="9" t="s">
+      <c r="A7" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="B7" s="10"/>
+      <c r="B7" s="9"/>
     </row>
     <row r="8" customFormat="false" ht="27.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="9" t="s">
+      <c r="A8" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="B8" s="10"/>
-      <c r="C8" s="11"/>
+      <c r="B8" s="9"/>
+      <c r="C8" s="10"/>
     </row>
     <row r="9" customFormat="false" ht="27.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="9" t="s">
+      <c r="A9" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="B9" s="10"/>
+      <c r="B9" s="9"/>
     </row>
     <row r="10" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="9" t="s">
+      <c r="A10" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="B10" s="10"/>
+      <c r="B10" s="9"/>
     </row>
     <row r="11" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="9" t="s">
+      <c r="A11" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="B11" s="10"/>
+      <c r="B11" s="9"/>
     </row>
     <row r="12" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="9" t="s">
+      <c r="A12" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="B12" s="10"/>
+      <c r="B12" s="9"/>
     </row>
     <row r="13" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="9" t="s">
+      <c r="A13" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="B13" s="12"/>
+      <c r="B13" s="11"/>
     </row>
     <row r="14" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="9" t="s">
+      <c r="A14" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="B14" s="10"/>
+      <c r="B14" s="9"/>
     </row>
     <row r="15" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="7" t="s">
@@ -1059,35 +1089,35 @@
       </c>
     </row>
     <row r="16" customFormat="false" ht="27.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A16" s="13" t="s">
+      <c r="A16" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="B16" s="13"/>
-      <c r="C16" s="13"/>
-      <c r="D16" s="13"/>
-      <c r="E16" s="13"/>
-      <c r="F16" s="13"/>
-      <c r="G16" s="13"/>
+      <c r="B16" s="12"/>
+      <c r="C16" s="12"/>
+      <c r="D16" s="12"/>
+      <c r="E16" s="12"/>
+      <c r="F16" s="12"/>
+      <c r="G16" s="12"/>
     </row>
     <row r="17" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A17" s="13" t="s">
+      <c r="A17" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="B17" s="13"/>
-      <c r="C17" s="13"/>
-      <c r="D17" s="13"/>
-      <c r="E17" s="13"/>
-      <c r="F17" s="13"/>
-      <c r="G17" s="13"/>
+      <c r="B17" s="12"/>
+      <c r="C17" s="12"/>
+      <c r="D17" s="12"/>
+      <c r="E17" s="12"/>
+      <c r="F17" s="12"/>
+      <c r="G17" s="12"/>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="14"/>
+      <c r="A18" s="13"/>
       <c r="B18" s="14"/>
-      <c r="C18" s="14"/>
-      <c r="D18" s="14"/>
-      <c r="E18" s="14"/>
-      <c r="F18" s="14"/>
-      <c r="G18" s="14"/>
+      <c r="C18" s="13"/>
+      <c r="D18" s="13"/>
+      <c r="E18" s="13"/>
+      <c r="F18" s="13"/>
+      <c r="G18" s="13"/>
     </row>
     <row r="19" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="15" t="s">
@@ -1147,13 +1177,13 @@
       <c r="A28" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="B28" s="10"/>
+      <c r="B28" s="9"/>
     </row>
     <row r="29" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="B29" s="10"/>
+      <c r="B29" s="9"/>
     </row>
     <row r="30" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="3" t="s">
@@ -1163,162 +1193,162 @@
     </row>
     <row r="31" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B31" s="19"/>
-      <c r="C31" s="19"/>
-      <c r="D31" s="19"/>
-      <c r="E31" s="19"/>
-      <c r="F31" s="19"/>
-      <c r="G31" s="19"/>
+      <c r="C31" s="20"/>
+      <c r="D31" s="20"/>
+      <c r="E31" s="20"/>
+      <c r="F31" s="20"/>
+      <c r="G31" s="20"/>
     </row>
     <row r="32" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="15" t="s">
         <v>30</v>
       </c>
-      <c r="B32" s="20"/>
-      <c r="C32" s="20"/>
-      <c r="D32" s="20"/>
-      <c r="E32" s="20"/>
-      <c r="F32" s="20"/>
-      <c r="G32" s="20"/>
+      <c r="B32" s="21"/>
+      <c r="C32" s="22"/>
+      <c r="D32" s="22"/>
+      <c r="E32" s="22"/>
+      <c r="F32" s="22"/>
+      <c r="G32" s="22"/>
     </row>
     <row r="33" customFormat="false" ht="19.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A33" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="B33" s="10"/>
-      <c r="C33" s="21" t="s">
+      <c r="B33" s="9"/>
+      <c r="C33" s="23" t="s">
         <v>32</v>
       </c>
-      <c r="D33" s="21"/>
-      <c r="E33" s="21"/>
-      <c r="F33" s="21"/>
-      <c r="G33" s="21"/>
+      <c r="D33" s="23"/>
+      <c r="E33" s="23"/>
+      <c r="F33" s="23"/>
+      <c r="G33" s="23"/>
     </row>
     <row r="34" customFormat="false" ht="19.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A34" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="B34" s="10"/>
-      <c r="C34" s="21" t="s">
+      <c r="B34" s="9"/>
+      <c r="C34" s="23" t="s">
         <v>34</v>
       </c>
-      <c r="D34" s="21"/>
-      <c r="E34" s="21"/>
-      <c r="F34" s="21"/>
-      <c r="G34" s="21"/>
-      <c r="H34" s="22"/>
+      <c r="D34" s="23"/>
+      <c r="E34" s="23"/>
+      <c r="F34" s="23"/>
+      <c r="G34" s="23"/>
+      <c r="H34" s="24"/>
     </row>
     <row r="35" customFormat="false" ht="19.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A35" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="B35" s="10"/>
-      <c r="C35" s="21" t="s">
+      <c r="B35" s="9"/>
+      <c r="C35" s="23" t="s">
         <v>36</v>
       </c>
-      <c r="D35" s="21"/>
-      <c r="E35" s="21"/>
-      <c r="F35" s="21"/>
-      <c r="G35" s="21"/>
+      <c r="D35" s="23"/>
+      <c r="E35" s="23"/>
+      <c r="F35" s="23"/>
+      <c r="G35" s="23"/>
     </row>
     <row r="36" customFormat="false" ht="19.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A36" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="B36" s="10"/>
-      <c r="C36" s="21" t="s">
+      <c r="B36" s="9"/>
+      <c r="C36" s="23" t="s">
         <v>36</v>
       </c>
-      <c r="D36" s="21"/>
-      <c r="E36" s="21"/>
-      <c r="F36" s="21"/>
-      <c r="G36" s="21"/>
+      <c r="D36" s="23"/>
+      <c r="E36" s="23"/>
+      <c r="F36" s="23"/>
+      <c r="G36" s="23"/>
     </row>
     <row r="37" customFormat="false" ht="39.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A37" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="B37" s="10"/>
-      <c r="C37" s="21" t="s">
+      <c r="B37" s="9"/>
+      <c r="C37" s="23" t="s">
         <v>34</v>
       </c>
-      <c r="D37" s="21"/>
-      <c r="E37" s="21"/>
-      <c r="F37" s="21"/>
-      <c r="G37" s="21"/>
+      <c r="D37" s="23"/>
+      <c r="E37" s="23"/>
+      <c r="F37" s="23"/>
+      <c r="G37" s="23"/>
     </row>
     <row r="38" customFormat="false" ht="19.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A38" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="B38" s="10"/>
-      <c r="C38" s="23" t="s">
+      <c r="B38" s="9"/>
+      <c r="C38" s="25" t="s">
         <v>40</v>
       </c>
-      <c r="D38" s="23"/>
-      <c r="E38" s="23"/>
-      <c r="F38" s="23"/>
-      <c r="G38" s="23"/>
+      <c r="D38" s="25"/>
+      <c r="E38" s="25"/>
+      <c r="F38" s="25"/>
+      <c r="G38" s="25"/>
     </row>
     <row r="39" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A39" s="13" t="s">
+      <c r="A39" s="12" t="s">
         <v>41</v>
       </c>
-      <c r="B39" s="13"/>
-      <c r="C39" s="13"/>
-      <c r="D39" s="13"/>
-      <c r="E39" s="13"/>
-      <c r="F39" s="13"/>
-      <c r="G39" s="13"/>
+      <c r="B39" s="12"/>
+      <c r="C39" s="12"/>
+      <c r="D39" s="12"/>
+      <c r="E39" s="12"/>
+      <c r="F39" s="12"/>
+      <c r="G39" s="12"/>
     </row>
     <row r="40" customFormat="false" ht="27.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="B40" s="10"/>
-      <c r="C40" s="24"/>
-      <c r="D40" s="24"/>
-      <c r="E40" s="24"/>
-      <c r="F40" s="24"/>
-      <c r="G40" s="24"/>
+      <c r="B40" s="9"/>
+      <c r="C40" s="26"/>
+      <c r="D40" s="26"/>
+      <c r="E40" s="26"/>
+      <c r="F40" s="26"/>
+      <c r="G40" s="26"/>
     </row>
     <row r="41" customFormat="false" ht="19.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A41" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="B41" s="10"/>
-      <c r="C41" s="21" t="s">
+      <c r="B41" s="9"/>
+      <c r="C41" s="23" t="s">
         <v>44</v>
       </c>
-      <c r="D41" s="21"/>
-      <c r="E41" s="21"/>
-      <c r="F41" s="21"/>
-      <c r="G41" s="21"/>
+      <c r="D41" s="23"/>
+      <c r="E41" s="23"/>
+      <c r="F41" s="23"/>
+      <c r="G41" s="23"/>
     </row>
     <row r="42" customFormat="false" ht="27.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A42" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="B42" s="10"/>
-      <c r="C42" s="21" t="s">
+      <c r="B42" s="9"/>
+      <c r="C42" s="23" t="s">
         <v>46</v>
       </c>
-      <c r="D42" s="21"/>
-      <c r="E42" s="21"/>
-      <c r="F42" s="21"/>
-      <c r="G42" s="21"/>
+      <c r="D42" s="23"/>
+      <c r="E42" s="23"/>
+      <c r="F42" s="23"/>
+      <c r="G42" s="23"/>
     </row>
     <row r="43" customFormat="false" ht="19.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A43" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="B43" s="10"/>
-      <c r="C43" s="21" t="s">
+      <c r="B43" s="9"/>
+      <c r="C43" s="23" t="s">
         <v>48</v>
       </c>
-      <c r="D43" s="21"/>
-      <c r="E43" s="21"/>
-      <c r="F43" s="21"/>
-      <c r="G43" s="21"/>
+      <c r="D43" s="23"/>
+      <c r="E43" s="23"/>
+      <c r="F43" s="23"/>
+      <c r="G43" s="23"/>
     </row>
     <row r="45" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="15" t="s">
@@ -1326,214 +1356,222 @@
       </c>
     </row>
     <row r="46" customFormat="false" ht="19.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A46" s="9" t="s">
+      <c r="A46" s="8" t="s">
         <v>50</v>
       </c>
       <c r="B46" s="18"/>
-      <c r="C46" s="21" t="s">
+      <c r="C46" s="23" t="s">
         <v>51</v>
       </c>
-      <c r="D46" s="21"/>
-      <c r="E46" s="21"/>
-      <c r="F46" s="21"/>
-      <c r="G46" s="21"/>
+      <c r="D46" s="23"/>
+      <c r="E46" s="23"/>
+      <c r="F46" s="23"/>
+      <c r="G46" s="23"/>
     </row>
     <row r="47" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A47" s="9" t="s">
+      <c r="A47" s="8" t="s">
         <v>52</v>
       </c>
       <c r="B47" s="17"/>
     </row>
     <row r="48" customFormat="false" ht="19.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A48" s="9" t="s">
+      <c r="A48" s="8" t="s">
         <v>53</v>
       </c>
       <c r="B48" s="18"/>
-      <c r="C48" s="21" t="s">
+      <c r="C48" s="23" t="s">
         <v>51</v>
       </c>
-      <c r="D48" s="21"/>
-      <c r="E48" s="21"/>
-      <c r="F48" s="21"/>
-      <c r="G48" s="21"/>
+      <c r="D48" s="23"/>
+      <c r="E48" s="23"/>
+      <c r="F48" s="23"/>
+      <c r="G48" s="23"/>
     </row>
     <row r="49" customFormat="false" ht="27.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A49" s="9" t="s">
+      <c r="A49" s="8" t="s">
         <v>54</v>
       </c>
       <c r="B49" s="17"/>
     </row>
     <row r="50" customFormat="false" ht="19.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A50" s="9" t="s">
+      <c r="A50" s="8" t="s">
         <v>55</v>
       </c>
       <c r="B50" s="17"/>
-      <c r="C50" s="21" t="s">
+      <c r="C50" s="23" t="s">
         <v>51</v>
       </c>
-      <c r="D50" s="21"/>
-      <c r="E50" s="21"/>
-      <c r="F50" s="21"/>
-      <c r="G50" s="21"/>
+      <c r="D50" s="23"/>
+      <c r="E50" s="23"/>
+      <c r="F50" s="23"/>
+      <c r="G50" s="23"/>
     </row>
     <row r="51" customFormat="false" ht="19.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A51" s="9" t="s">
+      <c r="A51" s="8" t="s">
         <v>56</v>
       </c>
       <c r="B51" s="17"/>
-      <c r="C51" s="21" t="s">
+      <c r="C51" s="23" t="s">
         <v>51</v>
       </c>
-      <c r="D51" s="21"/>
-      <c r="E51" s="21"/>
-      <c r="F51" s="21"/>
-      <c r="G51" s="21"/>
+      <c r="D51" s="23"/>
+      <c r="E51" s="23"/>
+      <c r="F51" s="23"/>
+      <c r="G51" s="23"/>
     </row>
     <row r="52" customFormat="false" ht="19.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A52" s="9" t="s">
+      <c r="A52" s="8" t="s">
         <v>57</v>
       </c>
       <c r="B52" s="17"/>
-      <c r="C52" s="21" t="s">
+      <c r="C52" s="23" t="s">
         <v>51</v>
       </c>
-      <c r="D52" s="21"/>
-      <c r="E52" s="21"/>
-      <c r="F52" s="21"/>
-      <c r="G52" s="21"/>
+      <c r="D52" s="23"/>
+      <c r="E52" s="23"/>
+      <c r="F52" s="23"/>
+      <c r="G52" s="23"/>
     </row>
     <row r="53" customFormat="false" ht="19.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A53" s="9" t="s">
+      <c r="A53" s="8" t="s">
         <v>58</v>
       </c>
-      <c r="B53" s="17"/>
-      <c r="C53" s="21" t="s">
+      <c r="B53" s="27" t="s">
+        <v>59</v>
+      </c>
+      <c r="C53" s="23" t="s">
         <v>51</v>
       </c>
-      <c r="D53" s="21"/>
-      <c r="E53" s="21"/>
-      <c r="F53" s="21"/>
-      <c r="G53" s="21"/>
+      <c r="D53" s="23"/>
+      <c r="E53" s="23"/>
+      <c r="F53" s="23"/>
+      <c r="G53" s="23"/>
     </row>
     <row r="54" customFormat="false" ht="19.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A54" s="9" t="s">
+      <c r="A54" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="B54" s="27" t="s">
         <v>59</v>
       </c>
-      <c r="B54" s="17"/>
-      <c r="C54" s="21" t="s">
+      <c r="C54" s="23" t="s">
         <v>51</v>
       </c>
-      <c r="D54" s="21"/>
-      <c r="E54" s="21"/>
-      <c r="F54" s="21"/>
-      <c r="G54" s="21"/>
+      <c r="D54" s="23"/>
+      <c r="E54" s="23"/>
+      <c r="F54" s="23"/>
+      <c r="G54" s="23"/>
     </row>
     <row r="55" customFormat="false" ht="19.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A55" s="9" t="s">
-        <v>60</v>
-      </c>
-      <c r="B55" s="17"/>
-      <c r="C55" s="21" t="s">
+      <c r="A55" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="B55" s="27" t="s">
+        <v>59</v>
+      </c>
+      <c r="C55" s="23" t="s">
         <v>51</v>
       </c>
-      <c r="D55" s="21"/>
-      <c r="E55" s="21"/>
-      <c r="F55" s="21"/>
-      <c r="G55" s="21"/>
+      <c r="D55" s="23"/>
+      <c r="E55" s="23"/>
+      <c r="F55" s="23"/>
+      <c r="G55" s="23"/>
     </row>
     <row r="56" customFormat="false" ht="19.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A56" s="9" t="s">
-        <v>61</v>
+      <c r="A56" s="8" t="s">
+        <v>62</v>
       </c>
       <c r="B56" s="17"/>
-      <c r="C56" s="21" t="s">
+      <c r="C56" s="23" t="s">
         <v>51</v>
       </c>
-      <c r="D56" s="21"/>
-      <c r="E56" s="21"/>
-      <c r="F56" s="21"/>
-      <c r="G56" s="21"/>
+      <c r="D56" s="23"/>
+      <c r="E56" s="23"/>
+      <c r="F56" s="23"/>
+      <c r="G56" s="23"/>
     </row>
     <row r="57" customFormat="false" ht="19.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A57" s="9" t="s">
-        <v>62</v>
+      <c r="A57" s="8" t="s">
+        <v>63</v>
       </c>
       <c r="B57" s="17"/>
-      <c r="C57" s="21" t="s">
+      <c r="C57" s="23" t="s">
         <v>51</v>
       </c>
-      <c r="D57" s="21"/>
-      <c r="E57" s="21"/>
-      <c r="F57" s="21"/>
-      <c r="G57" s="21"/>
+      <c r="D57" s="23"/>
+      <c r="E57" s="23"/>
+      <c r="F57" s="23"/>
+      <c r="G57" s="23"/>
     </row>
     <row r="58" customFormat="false" ht="19.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A58" s="9" t="s">
-        <v>63</v>
+      <c r="A58" s="8" t="s">
+        <v>64</v>
       </c>
       <c r="B58" s="17"/>
-      <c r="C58" s="21" t="s">
+      <c r="C58" s="23" t="s">
         <v>51</v>
       </c>
-      <c r="D58" s="21"/>
-      <c r="E58" s="21"/>
-      <c r="F58" s="21"/>
-      <c r="G58" s="21"/>
+      <c r="D58" s="23"/>
+      <c r="E58" s="23"/>
+      <c r="F58" s="23"/>
+      <c r="G58" s="23"/>
     </row>
     <row r="59" customFormat="false" ht="19.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A59" s="9" t="s">
-        <v>64</v>
+      <c r="A59" s="8" t="s">
+        <v>65</v>
       </c>
       <c r="B59" s="17"/>
-      <c r="C59" s="21" t="s">
+      <c r="C59" s="23" t="s">
         <v>51</v>
       </c>
-      <c r="D59" s="21"/>
-      <c r="E59" s="21"/>
-      <c r="F59" s="21"/>
-      <c r="G59" s="21"/>
+      <c r="D59" s="23"/>
+      <c r="E59" s="23"/>
+      <c r="F59" s="23"/>
+      <c r="G59" s="23"/>
     </row>
     <row r="60" customFormat="false" ht="27.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A60" s="9" t="s">
-        <v>65</v>
-      </c>
-      <c r="B60" s="17"/>
-      <c r="C60" s="21" t="s">
+      <c r="A60" s="8" t="s">
+        <v>66</v>
+      </c>
+      <c r="B60" s="27" t="s">
+        <v>59</v>
+      </c>
+      <c r="C60" s="23" t="s">
         <v>51</v>
       </c>
-      <c r="D60" s="21"/>
-      <c r="E60" s="21"/>
-      <c r="F60" s="21"/>
-      <c r="G60" s="21"/>
+      <c r="D60" s="23"/>
+      <c r="E60" s="23"/>
+      <c r="F60" s="23"/>
+      <c r="G60" s="23"/>
     </row>
     <row r="62" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="15" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="B63" s="10"/>
+        <v>68</v>
+      </c>
+      <c r="B63" s="9"/>
     </row>
     <row r="64" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A64" s="9" t="s">
-        <v>68</v>
-      </c>
-      <c r="B64" s="10"/>
+      <c r="A64" s="8" t="s">
+        <v>69</v>
+      </c>
+      <c r="B64" s="9"/>
     </row>
     <row r="65" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A65" s="9" t="s">
-        <v>69</v>
+      <c r="A65" s="8" t="s">
+        <v>70</v>
       </c>
       <c r="B65" s="17"/>
     </row>
     <row r="66" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A66" s="9" t="s">
-        <v>70</v>
-      </c>
-      <c r="B66" s="10"/>
+      <c r="A66" s="8" t="s">
+        <v>71</v>
+      </c>
+      <c r="B66" s="9"/>
     </row>
     <row r="67" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="3" t="s">
@@ -1549,308 +1587,308 @@
     </row>
     <row r="69" customFormat="false" ht="27.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A69" s="1" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="B69" s="18"/>
-      <c r="C69" s="25" t="s">
-        <v>72</v>
-      </c>
-      <c r="D69" s="25"/>
-      <c r="E69" s="25"/>
-      <c r="F69" s="25"/>
-      <c r="G69" s="25"/>
+      <c r="C69" s="28" t="s">
+        <v>73</v>
+      </c>
+      <c r="D69" s="28"/>
+      <c r="E69" s="28"/>
+      <c r="F69" s="28"/>
+      <c r="G69" s="28"/>
     </row>
     <row r="70" customFormat="false" ht="27.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="B70" s="10"/>
+        <v>74</v>
+      </c>
+      <c r="B70" s="9"/>
     </row>
     <row r="71" customFormat="false" ht="27.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A71" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="B71" s="10"/>
-      <c r="C71" s="26" t="s">
         <v>75</v>
       </c>
-      <c r="D71" s="26"/>
-      <c r="E71" s="26"/>
-      <c r="F71" s="26"/>
-      <c r="G71" s="26"/>
+      <c r="B71" s="9"/>
+      <c r="C71" s="29" t="s">
+        <v>76</v>
+      </c>
+      <c r="D71" s="29"/>
+      <c r="E71" s="29"/>
+      <c r="F71" s="29"/>
+      <c r="G71" s="29"/>
     </row>
     <row r="73" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="15" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A74" s="9" t="s">
-        <v>77</v>
+      <c r="A74" s="8" t="s">
+        <v>78</v>
       </c>
       <c r="B74" s="17"/>
     </row>
     <row r="75" customFormat="false" ht="27.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A75" s="9" t="s">
-        <v>78</v>
+      <c r="A75" s="8" t="s">
+        <v>79</v>
       </c>
       <c r="B75" s="17"/>
     </row>
     <row r="76" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A76" s="9" t="s">
-        <v>79</v>
+      <c r="A76" s="8" t="s">
+        <v>80</v>
       </c>
       <c r="B76" s="17"/>
     </row>
     <row r="77" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A77" s="9" t="s">
-        <v>80</v>
+      <c r="A77" s="8" t="s">
+        <v>81</v>
       </c>
       <c r="B77" s="17"/>
     </row>
     <row r="78" customFormat="false" ht="19.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A78" s="9" t="s">
-        <v>81</v>
+      <c r="A78" s="8" t="s">
+        <v>82</v>
       </c>
       <c r="B78" s="17"/>
-      <c r="C78" s="21" t="s">
+      <c r="C78" s="23" t="s">
         <v>51</v>
       </c>
-      <c r="D78" s="21"/>
-      <c r="E78" s="21"/>
-      <c r="F78" s="21"/>
-      <c r="G78" s="21"/>
+      <c r="D78" s="23"/>
+      <c r="E78" s="23"/>
+      <c r="F78" s="23"/>
+      <c r="G78" s="23"/>
     </row>
     <row r="79" customFormat="false" ht="27.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A79" s="9" t="s">
-        <v>82</v>
+      <c r="A79" s="8" t="s">
+        <v>83</v>
       </c>
       <c r="B79" s="17"/>
-      <c r="C79" s="21" t="s">
-        <v>83</v>
-      </c>
-      <c r="D79" s="21"/>
-      <c r="E79" s="21"/>
-      <c r="F79" s="21"/>
-      <c r="G79" s="21"/>
+      <c r="C79" s="23" t="s">
+        <v>84</v>
+      </c>
+      <c r="D79" s="23"/>
+      <c r="E79" s="23"/>
+      <c r="F79" s="23"/>
+      <c r="G79" s="23"/>
     </row>
     <row r="80" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A80" s="9" t="s">
-        <v>84</v>
+      <c r="A80" s="8" t="s">
+        <v>85</v>
       </c>
       <c r="B80" s="17"/>
     </row>
     <row r="81" customFormat="false" ht="19.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A81" s="9" t="s">
-        <v>85</v>
+      <c r="A81" s="8" t="s">
+        <v>86</v>
       </c>
       <c r="B81" s="17"/>
-      <c r="C81" s="21" t="s">
+      <c r="C81" s="23" t="s">
         <v>51</v>
       </c>
-      <c r="D81" s="21"/>
-      <c r="E81" s="21"/>
-      <c r="F81" s="21"/>
-      <c r="G81" s="21"/>
+      <c r="D81" s="23"/>
+      <c r="E81" s="23"/>
+      <c r="F81" s="23"/>
+      <c r="G81" s="23"/>
     </row>
     <row r="83" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A83" s="15" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
     </row>
     <row r="84" customFormat="false" ht="19.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A84" s="9" t="s">
-        <v>87</v>
+      <c r="A84" s="8" t="s">
+        <v>88</v>
       </c>
       <c r="B84" s="17"/>
-      <c r="C84" s="21" t="s">
+      <c r="C84" s="23" t="s">
         <v>51</v>
       </c>
-      <c r="D84" s="21"/>
-      <c r="E84" s="21"/>
-      <c r="F84" s="21"/>
-      <c r="G84" s="21"/>
+      <c r="D84" s="23"/>
+      <c r="E84" s="23"/>
+      <c r="F84" s="23"/>
+      <c r="G84" s="23"/>
     </row>
     <row r="85" customFormat="false" ht="27.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A85" s="9" t="s">
-        <v>88</v>
+      <c r="A85" s="8" t="s">
+        <v>89</v>
       </c>
       <c r="B85" s="17"/>
-      <c r="C85" s="21" t="s">
+      <c r="C85" s="23" t="s">
         <v>51</v>
       </c>
-      <c r="D85" s="21"/>
-      <c r="E85" s="21"/>
-      <c r="F85" s="21"/>
-      <c r="G85" s="21"/>
+      <c r="D85" s="23"/>
+      <c r="E85" s="23"/>
+      <c r="F85" s="23"/>
+      <c r="G85" s="23"/>
     </row>
     <row r="86" customFormat="false" ht="19.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A86" s="9" t="s">
-        <v>89</v>
+      <c r="A86" s="8" t="s">
+        <v>90</v>
       </c>
       <c r="B86" s="17"/>
-      <c r="C86" s="21" t="s">
+      <c r="C86" s="23" t="s">
         <v>51</v>
       </c>
-      <c r="D86" s="21"/>
-      <c r="E86" s="21"/>
-      <c r="F86" s="21"/>
-      <c r="G86" s="21"/>
+      <c r="D86" s="23"/>
+      <c r="E86" s="23"/>
+      <c r="F86" s="23"/>
+      <c r="G86" s="23"/>
     </row>
     <row r="87" customFormat="false" ht="19.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A87" s="9" t="s">
-        <v>90</v>
+      <c r="A87" s="8" t="s">
+        <v>91</v>
       </c>
       <c r="B87" s="17"/>
-      <c r="C87" s="21" t="s">
+      <c r="C87" s="23" t="s">
         <v>51</v>
       </c>
-      <c r="D87" s="21"/>
-      <c r="E87" s="21"/>
-      <c r="F87" s="21"/>
-      <c r="G87" s="21"/>
+      <c r="D87" s="23"/>
+      <c r="E87" s="23"/>
+      <c r="F87" s="23"/>
+      <c r="G87" s="23"/>
     </row>
     <row r="88" customFormat="false" ht="19.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A88" s="9" t="s">
-        <v>91</v>
+      <c r="A88" s="8" t="s">
+        <v>92</v>
       </c>
       <c r="B88" s="17"/>
-      <c r="C88" s="21" t="s">
+      <c r="C88" s="23" t="s">
         <v>51</v>
       </c>
-      <c r="D88" s="21"/>
-      <c r="E88" s="21"/>
-      <c r="F88" s="21"/>
-      <c r="G88" s="21"/>
+      <c r="D88" s="23"/>
+      <c r="E88" s="23"/>
+      <c r="F88" s="23"/>
+      <c r="G88" s="23"/>
     </row>
     <row r="90" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A90" s="15" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
     </row>
     <row r="91" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A91" s="9" t="s">
-        <v>93</v>
+      <c r="A91" s="8" t="s">
+        <v>94</v>
       </c>
       <c r="B91" s="17"/>
     </row>
     <row r="92" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A92" s="9" t="s">
-        <v>94</v>
+      <c r="A92" s="8" t="s">
+        <v>95</v>
       </c>
       <c r="B92" s="17"/>
     </row>
     <row r="93" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A93" s="9" t="s">
-        <v>95</v>
+      <c r="A93" s="8" t="s">
+        <v>96</v>
       </c>
       <c r="B93" s="17"/>
     </row>
     <row r="94" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A94" s="9" t="s">
-        <v>96</v>
+      <c r="A94" s="8" t="s">
+        <v>97</v>
       </c>
       <c r="B94" s="17"/>
     </row>
     <row r="95" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A95" s="9" t="s">
-        <v>97</v>
+      <c r="A95" s="8" t="s">
+        <v>98</v>
       </c>
       <c r="B95" s="17"/>
     </row>
     <row r="96" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A96" s="9" t="s">
-        <v>98</v>
+      <c r="A96" s="8" t="s">
+        <v>99</v>
       </c>
       <c r="B96" s="17"/>
     </row>
     <row r="97" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A97" s="9" t="s">
-        <v>99</v>
+      <c r="A97" s="8" t="s">
+        <v>100</v>
       </c>
       <c r="B97" s="17"/>
     </row>
     <row r="98" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A98" s="1" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="B98" s="17"/>
     </row>
     <row r="99" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A99" s="1" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="B99" s="17"/>
     </row>
     <row r="100" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A100" s="1" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="B100" s="17"/>
     </row>
     <row r="101" customFormat="false" ht="27.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A101" s="1" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="B101" s="17"/>
     </row>
     <row r="102" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A102" s="1" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="B102" s="17"/>
     </row>
     <row r="103" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A103" s="1" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="B103" s="17"/>
     </row>
     <row r="104" customFormat="false" ht="39.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A104" s="1" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="B104" s="17"/>
     </row>
     <row r="105" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A105" s="9" t="s">
-        <v>107</v>
+      <c r="A105" s="8" t="s">
+        <v>108</v>
       </c>
       <c r="B105" s="17"/>
     </row>
     <row r="106" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A106" s="9" t="s">
-        <v>108</v>
+      <c r="A106" s="8" t="s">
+        <v>109</v>
       </c>
       <c r="B106" s="17"/>
     </row>
     <row r="107" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A107" s="9" t="s">
-        <v>109</v>
+      <c r="A107" s="8" t="s">
+        <v>110</v>
       </c>
       <c r="B107" s="17"/>
     </row>
     <row r="108" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A108" s="9" t="s">
-        <v>110</v>
+      <c r="A108" s="8" t="s">
+        <v>111</v>
       </c>
       <c r="B108" s="17"/>
     </row>
     <row r="109" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A109" s="9" t="s">
-        <v>111</v>
+      <c r="A109" s="8" t="s">
+        <v>112</v>
       </c>
       <c r="B109" s="17"/>
     </row>
     <row r="110" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A110" s="9" t="s">
-        <v>112</v>
+      <c r="A110" s="8" t="s">
+        <v>113</v>
       </c>
       <c r="B110" s="17"/>
     </row>
     <row r="111" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A111" s="9" t="s">
-        <v>113</v>
+      <c r="A111" s="8" t="s">
+        <v>114</v>
       </c>
       <c r="B111" s="17"/>
     </row>

</xml_diff>

<commit_message>
evaluation adherence to requirements and improvements
</commit_message>
<xml_diff>
--- a/report/checklist.xlsx
+++ b/report/checklist.xlsx
@@ -765,7 +765,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="29">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -834,14 +834,14 @@
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="165" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="165" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="165" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -872,10 +872,6 @@
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
@@ -977,11 +973,11 @@
   </sheetPr>
   <dimension ref="A1:H111"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A43" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A60" activeCellId="0" sqref="A60"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A10" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A21" activeCellId="0" sqref="A21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.8515625" defaultRowHeight="19.7" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.84375" defaultRowHeight="19.7" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="70.62"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="2" width="6.06"/>
@@ -1129,21 +1125,21 @@
       <c r="A20" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="B20" s="17"/>
+      <c r="B20" s="9"/>
     </row>
     <row r="21" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="B21" s="17"/>
+      <c r="B21" s="9"/>
     </row>
     <row r="22" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="B22" s="17"/>
-    </row>
-    <row r="23" customFormat="false" ht="27.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B22" s="9"/>
+    </row>
+    <row r="23" customFormat="false" ht="29.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="3" t="s">
         <v>22</v>
       </c>
@@ -1153,25 +1149,25 @@
       <c r="A24" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="B24" s="18"/>
+      <c r="B24" s="9"/>
     </row>
     <row r="25" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="B25" s="17"/>
+      <c r="B25" s="18"/>
     </row>
     <row r="26" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="B26" s="17"/>
+      <c r="B26" s="18"/>
     </row>
     <row r="27" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="B27" s="17"/>
+      <c r="B27" s="18"/>
     </row>
     <row r="28" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="3" t="s">
@@ -1189,7 +1185,7 @@
       <c r="A30" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="B30" s="17"/>
+      <c r="B30" s="18"/>
     </row>
     <row r="31" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B31" s="19"/>
@@ -1359,7 +1355,7 @@
       <c r="A46" s="8" t="s">
         <v>50</v>
       </c>
-      <c r="B46" s="18"/>
+      <c r="B46" s="17"/>
       <c r="C46" s="23" t="s">
         <v>51</v>
       </c>
@@ -1372,13 +1368,13 @@
       <c r="A47" s="8" t="s">
         <v>52</v>
       </c>
-      <c r="B47" s="17"/>
+      <c r="B47" s="18"/>
     </row>
     <row r="48" customFormat="false" ht="19.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A48" s="8" t="s">
         <v>53</v>
       </c>
-      <c r="B48" s="18"/>
+      <c r="B48" s="17"/>
       <c r="C48" s="23" t="s">
         <v>51</v>
       </c>
@@ -1391,13 +1387,13 @@
       <c r="A49" s="8" t="s">
         <v>54</v>
       </c>
-      <c r="B49" s="17"/>
+      <c r="B49" s="18"/>
     </row>
     <row r="50" customFormat="false" ht="19.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A50" s="8" t="s">
         <v>55</v>
       </c>
-      <c r="B50" s="17"/>
+      <c r="B50" s="18"/>
       <c r="C50" s="23" t="s">
         <v>51</v>
       </c>
@@ -1410,7 +1406,7 @@
       <c r="A51" s="8" t="s">
         <v>56</v>
       </c>
-      <c r="B51" s="17"/>
+      <c r="B51" s="18"/>
       <c r="C51" s="23" t="s">
         <v>51</v>
       </c>
@@ -1423,7 +1419,7 @@
       <c r="A52" s="8" t="s">
         <v>57</v>
       </c>
-      <c r="B52" s="17"/>
+      <c r="B52" s="18"/>
       <c r="C52" s="23" t="s">
         <v>51</v>
       </c>
@@ -1436,7 +1432,7 @@
       <c r="A53" s="8" t="s">
         <v>58</v>
       </c>
-      <c r="B53" s="27" t="s">
+      <c r="B53" s="16" t="s">
         <v>59</v>
       </c>
       <c r="C53" s="23" t="s">
@@ -1451,7 +1447,7 @@
       <c r="A54" s="8" t="s">
         <v>60</v>
       </c>
-      <c r="B54" s="27" t="s">
+      <c r="B54" s="16" t="s">
         <v>59</v>
       </c>
       <c r="C54" s="23" t="s">
@@ -1466,7 +1462,7 @@
       <c r="A55" s="8" t="s">
         <v>61</v>
       </c>
-      <c r="B55" s="27" t="s">
+      <c r="B55" s="16" t="s">
         <v>59</v>
       </c>
       <c r="C55" s="23" t="s">
@@ -1481,7 +1477,7 @@
       <c r="A56" s="8" t="s">
         <v>62</v>
       </c>
-      <c r="B56" s="17"/>
+      <c r="B56" s="18"/>
       <c r="C56" s="23" t="s">
         <v>51</v>
       </c>
@@ -1494,7 +1490,7 @@
       <c r="A57" s="8" t="s">
         <v>63</v>
       </c>
-      <c r="B57" s="17"/>
+      <c r="B57" s="18"/>
       <c r="C57" s="23" t="s">
         <v>51</v>
       </c>
@@ -1507,7 +1503,7 @@
       <c r="A58" s="8" t="s">
         <v>64</v>
       </c>
-      <c r="B58" s="17"/>
+      <c r="B58" s="18"/>
       <c r="C58" s="23" t="s">
         <v>51</v>
       </c>
@@ -1520,7 +1516,7 @@
       <c r="A59" s="8" t="s">
         <v>65</v>
       </c>
-      <c r="B59" s="17"/>
+      <c r="B59" s="18"/>
       <c r="C59" s="23" t="s">
         <v>51</v>
       </c>
@@ -1533,7 +1529,7 @@
       <c r="A60" s="8" t="s">
         <v>66</v>
       </c>
-      <c r="B60" s="27" t="s">
+      <c r="B60" s="16" t="s">
         <v>59</v>
       </c>
       <c r="C60" s="23" t="s">
@@ -1565,7 +1561,7 @@
       <c r="A65" s="8" t="s">
         <v>70</v>
       </c>
-      <c r="B65" s="17"/>
+      <c r="B65" s="18"/>
     </row>
     <row r="66" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="8" t="s">
@@ -1577,26 +1573,26 @@
       <c r="A67" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="B67" s="17"/>
+      <c r="B67" s="18"/>
     </row>
     <row r="68" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="B68" s="17"/>
+      <c r="B68" s="18"/>
     </row>
     <row r="69" customFormat="false" ht="27.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A69" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="B69" s="18"/>
-      <c r="C69" s="28" t="s">
+      <c r="B69" s="17"/>
+      <c r="C69" s="27" t="s">
         <v>73</v>
       </c>
-      <c r="D69" s="28"/>
-      <c r="E69" s="28"/>
-      <c r="F69" s="28"/>
-      <c r="G69" s="28"/>
+      <c r="D69" s="27"/>
+      <c r="E69" s="27"/>
+      <c r="F69" s="27"/>
+      <c r="G69" s="27"/>
     </row>
     <row r="70" customFormat="false" ht="27.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="1" t="s">
@@ -1609,13 +1605,13 @@
         <v>75</v>
       </c>
       <c r="B71" s="9"/>
-      <c r="C71" s="29" t="s">
+      <c r="C71" s="28" t="s">
         <v>76</v>
       </c>
-      <c r="D71" s="29"/>
-      <c r="E71" s="29"/>
-      <c r="F71" s="29"/>
-      <c r="G71" s="29"/>
+      <c r="D71" s="28"/>
+      <c r="E71" s="28"/>
+      <c r="F71" s="28"/>
+      <c r="G71" s="28"/>
     </row>
     <row r="73" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="15" t="s">
@@ -1626,31 +1622,31 @@
       <c r="A74" s="8" t="s">
         <v>78</v>
       </c>
-      <c r="B74" s="17"/>
+      <c r="B74" s="18"/>
     </row>
     <row r="75" customFormat="false" ht="27.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="8" t="s">
         <v>79</v>
       </c>
-      <c r="B75" s="17"/>
+      <c r="B75" s="18"/>
     </row>
     <row r="76" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="8" t="s">
         <v>80</v>
       </c>
-      <c r="B76" s="17"/>
+      <c r="B76" s="18"/>
     </row>
     <row r="77" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="8" t="s">
         <v>81</v>
       </c>
-      <c r="B77" s="17"/>
+      <c r="B77" s="18"/>
     </row>
     <row r="78" customFormat="false" ht="19.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A78" s="8" t="s">
         <v>82</v>
       </c>
-      <c r="B78" s="17"/>
+      <c r="B78" s="18"/>
       <c r="C78" s="23" t="s">
         <v>51</v>
       </c>
@@ -1663,7 +1659,7 @@
       <c r="A79" s="8" t="s">
         <v>83</v>
       </c>
-      <c r="B79" s="17"/>
+      <c r="B79" s="18"/>
       <c r="C79" s="23" t="s">
         <v>84</v>
       </c>
@@ -1676,13 +1672,13 @@
       <c r="A80" s="8" t="s">
         <v>85</v>
       </c>
-      <c r="B80" s="17"/>
+      <c r="B80" s="18"/>
     </row>
     <row r="81" customFormat="false" ht="19.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A81" s="8" t="s">
         <v>86</v>
       </c>
-      <c r="B81" s="17"/>
+      <c r="B81" s="18"/>
       <c r="C81" s="23" t="s">
         <v>51</v>
       </c>
@@ -1700,7 +1696,7 @@
       <c r="A84" s="8" t="s">
         <v>88</v>
       </c>
-      <c r="B84" s="17"/>
+      <c r="B84" s="18"/>
       <c r="C84" s="23" t="s">
         <v>51</v>
       </c>
@@ -1713,7 +1709,7 @@
       <c r="A85" s="8" t="s">
         <v>89</v>
       </c>
-      <c r="B85" s="17"/>
+      <c r="B85" s="18"/>
       <c r="C85" s="23" t="s">
         <v>51</v>
       </c>
@@ -1726,7 +1722,7 @@
       <c r="A86" s="8" t="s">
         <v>90</v>
       </c>
-      <c r="B86" s="17"/>
+      <c r="B86" s="18"/>
       <c r="C86" s="23" t="s">
         <v>51</v>
       </c>
@@ -1739,7 +1735,7 @@
       <c r="A87" s="8" t="s">
         <v>91</v>
       </c>
-      <c r="B87" s="17"/>
+      <c r="B87" s="18"/>
       <c r="C87" s="23" t="s">
         <v>51</v>
       </c>
@@ -1752,7 +1748,7 @@
       <c r="A88" s="8" t="s">
         <v>92</v>
       </c>
-      <c r="B88" s="17"/>
+      <c r="B88" s="18"/>
       <c r="C88" s="23" t="s">
         <v>51</v>
       </c>
@@ -1770,127 +1766,127 @@
       <c r="A91" s="8" t="s">
         <v>94</v>
       </c>
-      <c r="B91" s="17"/>
+      <c r="B91" s="18"/>
     </row>
     <row r="92" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A92" s="8" t="s">
         <v>95</v>
       </c>
-      <c r="B92" s="17"/>
+      <c r="B92" s="18"/>
     </row>
     <row r="93" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A93" s="8" t="s">
         <v>96</v>
       </c>
-      <c r="B93" s="17"/>
+      <c r="B93" s="18"/>
     </row>
     <row r="94" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A94" s="8" t="s">
         <v>97</v>
       </c>
-      <c r="B94" s="17"/>
+      <c r="B94" s="18"/>
     </row>
     <row r="95" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A95" s="8" t="s">
         <v>98</v>
       </c>
-      <c r="B95" s="17"/>
+      <c r="B95" s="18"/>
     </row>
     <row r="96" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A96" s="8" t="s">
         <v>99</v>
       </c>
-      <c r="B96" s="17"/>
+      <c r="B96" s="18"/>
     </row>
     <row r="97" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A97" s="8" t="s">
         <v>100</v>
       </c>
-      <c r="B97" s="17"/>
+      <c r="B97" s="18"/>
     </row>
     <row r="98" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A98" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="B98" s="17"/>
+      <c r="B98" s="18"/>
     </row>
     <row r="99" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A99" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="B99" s="17"/>
+      <c r="B99" s="18"/>
     </row>
     <row r="100" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A100" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="B100" s="17"/>
+      <c r="B100" s="18"/>
     </row>
     <row r="101" customFormat="false" ht="27.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A101" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="B101" s="17"/>
+      <c r="B101" s="18"/>
     </row>
     <row r="102" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A102" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="B102" s="17"/>
+      <c r="B102" s="18"/>
     </row>
     <row r="103" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A103" s="1" t="s">
         <v>106</v>
       </c>
-      <c r="B103" s="17"/>
+      <c r="B103" s="18"/>
     </row>
     <row r="104" customFormat="false" ht="39.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A104" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="B104" s="17"/>
+      <c r="B104" s="18"/>
     </row>
     <row r="105" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A105" s="8" t="s">
         <v>108</v>
       </c>
-      <c r="B105" s="17"/>
+      <c r="B105" s="18"/>
     </row>
     <row r="106" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A106" s="8" t="s">
         <v>109</v>
       </c>
-      <c r="B106" s="17"/>
+      <c r="B106" s="18"/>
     </row>
     <row r="107" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A107" s="8" t="s">
         <v>110</v>
       </c>
-      <c r="B107" s="17"/>
+      <c r="B107" s="18"/>
     </row>
     <row r="108" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A108" s="8" t="s">
         <v>111</v>
       </c>
-      <c r="B108" s="17"/>
+      <c r="B108" s="18"/>
     </row>
     <row r="109" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A109" s="8" t="s">
         <v>112</v>
       </c>
-      <c r="B109" s="17"/>
+      <c r="B109" s="18"/>
     </row>
     <row r="110" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A110" s="8" t="s">
         <v>113</v>
       </c>
-      <c r="B110" s="17"/>
+      <c r="B110" s="18"/>
     </row>
     <row r="111" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A111" s="8" t="s">
         <v>114</v>
       </c>
-      <c r="B111" s="17"/>
+      <c r="B111" s="18"/>
     </row>
   </sheetData>
   <mergeCells count="36">
@@ -1931,7 +1927,7 @@
     <mergeCell ref="C87:G87"/>
     <mergeCell ref="C88:G88"/>
   </mergeCells>
-  <conditionalFormatting sqref="B19:B38 B2:B15 B40:B1048576">
+  <conditionalFormatting sqref="B2:B15 B40:B1048576 B19:B38">
     <cfRule type="containsText" priority="2" operator="containsText" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="ü" dxfId="0">
       <formula>NOT(ISERROR(SEARCH("ü",B2)))</formula>
     </cfRule>

</xml_diff>